<commit_message>
Improved figures, improved data tables
</commit_message>
<xml_diff>
--- a/data/03_processed/combined_df_long.xlsx
+++ b/data/03_processed/combined_df_long.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S182"/>
+  <dimension ref="A1:U182"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,10 +516,20 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>wd_start</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ht_start</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>wd_rel</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>ht_rel</t>
         </is>
@@ -581,7 +591,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F693dcac4-051b-2abf-6010-9d6658109d60-20220423_142023.jpg?Expires=1652401055941&amp;KeyName=labelbox-assets-key-3&amp;Signature=uPSalbR6kGmx_R0vKCHzXwSKxwE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F693dcac4-051b-2abf-6010-9d6658109d60-20220423_142023.jpg?Expires=1652726495781&amp;KeyName=labelbox-assets-key-3&amp;Signature=CMzlw-jIUsdacoyYKAHy4Ro42g4</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -596,9 +606,15 @@
         <v>261</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>585</v>
       </c>
       <c r="S2" t="n">
+        <v>2470</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -658,7 +674,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8ee2e0aa-418b-83b4-7751-872f756ef0d8-20220423_142031.jpg?Expires=1652401055941&amp;KeyName=labelbox-assets-key-3&amp;Signature=kn9O3uXELzEtLR5nhvtkQK2SYN0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8ee2e0aa-418b-83b4-7751-872f756ef0d8-20220423_142031.jpg?Expires=1652726495781&amp;KeyName=labelbox-assets-key-3&amp;Signature=ha96ekv1nLy4otnDeRpIdHDsN4w</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -673,9 +689,15 @@
         <v>287</v>
       </c>
       <c r="R3" t="n">
+        <v>614</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2470</v>
+      </c>
+      <c r="T3" t="n">
         <v>0.2607003891050583</v>
       </c>
-      <c r="S3" t="n">
+      <c r="U3" t="n">
         <v>-0.09961685823754785</v>
       </c>
     </row>
@@ -735,7 +757,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdea7e873-6eae-0208-0540-a8f8f9c187cc-20220423_142049.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=ph4I6G6UdIL0IrujIouF1_V5nKo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdea7e873-6eae-0208-0540-a8f8f9c187cc-20220423_142049.jpg?Expires=1652726495781&amp;KeyName=labelbox-assets-key-3&amp;Signature=YEQD9grwHN05smnQ443IwixYDVw</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -750,9 +772,15 @@
         <v>252</v>
       </c>
       <c r="R4" t="n">
+        <v>655</v>
+      </c>
+      <c r="S4" t="n">
+        <v>2464</v>
+      </c>
+      <c r="T4" t="n">
         <v>0.5330739299610895</v>
       </c>
-      <c r="S4" t="n">
+      <c r="U4" t="n">
         <v>0.03448275862068961</v>
       </c>
     </row>
@@ -812,7 +840,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F943cab09-0c2c-1220-e6f0-d5134abc698f-20220423_142054.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=St4qDHfVxJOoCXkfc98j1V34aTE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F943cab09-0c2c-1220-e6f0-d5134abc698f-20220423_142054.jpg?Expires=1652726495781&amp;KeyName=labelbox-assets-key-3&amp;Signature=VMplpXz8tl6md1wlNbL4jAhZXGg</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -827,9 +855,15 @@
         <v>250</v>
       </c>
       <c r="R5" t="n">
+        <v>670</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2463</v>
+      </c>
+      <c r="T5" t="n">
         <v>0.6498054474708171</v>
       </c>
-      <c r="S5" t="n">
+      <c r="U5" t="n">
         <v>0.04214559386973182</v>
       </c>
     </row>
@@ -889,7 +923,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa92fa255-d1a8-f14f-74bf-720424b2eec3-20220423_142100.jpg?Expires=1652401055940&amp;KeyName=labelbox-assets-key-3&amp;Signature=Dyi3bYYGeImEXNXcrz9tx1XpRiE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa92fa255-d1a8-f14f-74bf-720424b2eec3-20220423_142100.jpg?Expires=1652726495780&amp;KeyName=labelbox-assets-key-3&amp;Signature=k0syH1uS3Uz1VQ674_-xl7r4Lf8</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -904,9 +938,15 @@
         <v>361</v>
       </c>
       <c r="R6" t="n">
+        <v>672</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2470</v>
+      </c>
+      <c r="T6" t="n">
         <v>0.7470817120622568</v>
       </c>
-      <c r="S6" t="n">
+      <c r="U6" t="n">
         <v>-0.3831417624521072</v>
       </c>
     </row>
@@ -966,7 +1006,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F92ace430-e51d-d85c-70fc-3d616430c490-20220423_142108.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=QXS5ptgDILdhYQIS9ZnYwntYhtA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F92ace430-e51d-d85c-70fc-3d616430c490-20220423_142108.jpg?Expires=1652726495781&amp;KeyName=labelbox-assets-key-3&amp;Signature=WUsZJ8OrK-_v_Q2egODvV2DoVmc</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -981,9 +1021,15 @@
         <v>140</v>
       </c>
       <c r="R7" t="n">
+        <v>681</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2468</v>
+      </c>
+      <c r="T7" t="n">
         <v>0.8287937743190661</v>
       </c>
-      <c r="S7" t="n">
+      <c r="U7" t="n">
         <v>0.4636015325670498</v>
       </c>
     </row>
@@ -1043,7 +1089,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7514df0f-b16f-d5d0-6915-77662032c57f-20220423_143310.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=9N5APaNkB0ezYBR6il0NCuNak0Q</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7514df0f-b16f-d5d0-6915-77662032c57f-20220423_143310.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=aflLd6xli7KZGMuHMUsTSpXryX8</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1058,9 +1104,15 @@
         <v>243</v>
       </c>
       <c r="R8" t="n">
-        <v>0</v>
+        <v>685</v>
       </c>
       <c r="S8" t="n">
+        <v>2435</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1120,7 +1172,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fbdf002ed-162b-b204-ca31-16d8b19f1bb8-20220423_143324.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=I09aO4M51LZcP0mqemDXh9GrQR0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fbdf002ed-162b-b204-ca31-16d8b19f1bb8-20220423_143324.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=p9pfWXmjkUDSGDSiatxrmz_U4L4</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1135,9 +1187,15 @@
         <v>221</v>
       </c>
       <c r="R9" t="n">
+        <v>729</v>
+      </c>
+      <c r="S9" t="n">
+        <v>2433</v>
+      </c>
+      <c r="T9" t="n">
         <v>0.2418772563176895</v>
       </c>
-      <c r="S9" t="n">
+      <c r="U9" t="n">
         <v>0.09053497942386834</v>
       </c>
     </row>
@@ -1197,7 +1255,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fccfdcb1f-5ee4-34cb-bce3-dd7235989bbc-20220423_143336.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=LWmwEzoQiDhmrRfNrkhcSk8IInc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fccfdcb1f-5ee4-34cb-bce3-dd7235989bbc-20220423_143336.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=Tctz2FWW4Z9NX0MLbYrL9LEKGLQ</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1212,9 +1270,15 @@
         <v>192</v>
       </c>
       <c r="R10" t="n">
+        <v>762</v>
+      </c>
+      <c r="S10" t="n">
+        <v>2433</v>
+      </c>
+      <c r="T10" t="n">
         <v>0.4729241877256317</v>
       </c>
-      <c r="S10" t="n">
+      <c r="U10" t="n">
         <v>0.2098765432098766</v>
       </c>
     </row>
@@ -1274,7 +1338,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8843bee5-e78e-59bd-09a0-83cb23856efc-20220423_143346.jpg?Expires=1652401055942&amp;KeyName=labelbox-assets-key-3&amp;Signature=7utZtb4fTFET-SgBK5sG3SiMfMw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8843bee5-e78e-59bd-09a0-83cb23856efc-20220423_143346.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=5iL5fesHxzH8wa26X3xxLQFjnp8</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1289,9 +1353,15 @@
         <v>236</v>
       </c>
       <c r="R11" t="n">
+        <v>774</v>
+      </c>
+      <c r="S11" t="n">
+        <v>2439</v>
+      </c>
+      <c r="T11" t="n">
         <v>0.5812274368231047</v>
       </c>
-      <c r="S11" t="n">
+      <c r="U11" t="n">
         <v>0.0288065843621399</v>
       </c>
     </row>
@@ -1351,7 +1421,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8270c425-c0f3-7b72-baa6-a2fd71fc5753-20220423_143355.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=4BHUuWeuWeLOJF0yLa_qEEf9Sbg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8270c425-c0f3-7b72-baa6-a2fd71fc5753-20220423_143355.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=H18L3GrXW8YCU_zoA799ofbNJRc</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -1366,9 +1436,15 @@
         <v>145</v>
       </c>
       <c r="R12" t="n">
+        <v>792</v>
+      </c>
+      <c r="S12" t="n">
+        <v>2437</v>
+      </c>
+      <c r="T12" t="n">
         <v>0.6967509025270758</v>
       </c>
-      <c r="S12" t="n">
+      <c r="U12" t="n">
         <v>0.4032921810699589</v>
       </c>
     </row>
@@ -1428,7 +1504,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4b622045-5700-ce69-9810-0b2571595e2a-20220423_143401.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=1vl0zrb_Dg35373wHdK8EMSek8E</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4b622045-5700-ce69-9810-0b2571595e2a-20220423_143401.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=6R_4tW6VEo_d4XQM7Lr0B7ymbwQ</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -1443,9 +1519,15 @@
         <v>121</v>
       </c>
       <c r="R13" t="n">
+        <v>796</v>
+      </c>
+      <c r="S13" t="n">
+        <v>2439</v>
+      </c>
+      <c r="T13" t="n">
         <v>0.7581227436823105</v>
       </c>
-      <c r="S13" t="n">
+      <c r="U13" t="n">
         <v>0.5020576131687242</v>
       </c>
     </row>
@@ -1505,7 +1587,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6d1fb1b4-5386-82e4-966f-d844f324b3a9-20220423_143756.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=zrIdlybYzA3XOzT6ON1wE7LDXMA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6d1fb1b4-5386-82e4-966f-d844f324b3a9-20220423_143756.jpg?Expires=1652726495782&amp;KeyName=labelbox-assets-key-3&amp;Signature=rj6gOwTuC3FgsD3q1PVQ3azrR8Q</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -1520,9 +1602,15 @@
         <v>222</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>866</v>
       </c>
       <c r="S14" t="n">
+        <v>2432</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1582,7 +1670,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3127d07-4bb7-9be8-5cd7-d8c6e6ef23ab-20220423_143810.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=yD3T67B9P8wzF8z-uIw3OTTE0dU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3127d07-4bb7-9be8-5cd7-d8c6e6ef23ab-20220423_143810.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=R2gaI5s6HNKvVa4I8mPmZdF_2EE</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1597,9 +1685,15 @@
         <v>169</v>
       </c>
       <c r="R15" t="n">
+        <v>849</v>
+      </c>
+      <c r="S15" t="n">
+        <v>2460</v>
+      </c>
+      <c r="T15" t="n">
         <v>0.1321585903083701</v>
       </c>
-      <c r="S15" t="n">
+      <c r="U15" t="n">
         <v>0.2387387387387387</v>
       </c>
     </row>
@@ -1659,7 +1753,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F63112db6-64f3-d7c4-21a6-83e8ee92da07-20220423_143815.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=hUs_Dq_jyFOUTpjvn2-rvw3D1s0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F63112db6-64f3-d7c4-21a6-83e8ee92da07-20220423_143815.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=C0dOAL4m-ZTwX2IbX5mjwQlsya0</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1674,9 +1768,15 @@
         <v>160</v>
       </c>
       <c r="R16" t="n">
+        <v>878</v>
+      </c>
+      <c r="S16" t="n">
+        <v>2432</v>
+      </c>
+      <c r="T16" t="n">
         <v>0.4096916299559471</v>
       </c>
-      <c r="S16" t="n">
+      <c r="U16" t="n">
         <v>0.2792792792792793</v>
       </c>
     </row>
@@ -1736,7 +1836,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5918f5a-1363-7347-cd34-924205589432-20220423_143824.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=fvljhnKWdfUX2N75OjUmH7_Zyro</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5918f5a-1363-7347-cd34-924205589432-20220423_143824.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=f483UahfLnf3KOsscgkStz9H4p8</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1751,9 +1851,15 @@
         <v>166</v>
       </c>
       <c r="R17" t="n">
+        <v>900</v>
+      </c>
+      <c r="S17" t="n">
+        <v>2400</v>
+      </c>
+      <c r="T17" t="n">
         <v>0.6387665198237886</v>
       </c>
-      <c r="S17" t="n">
+      <c r="U17" t="n">
         <v>0.2522522522522522</v>
       </c>
     </row>
@@ -1813,7 +1919,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F388a3201-70c0-2ad9-9d16-f1ae9c146436-20220423_143829.jpg?Expires=1652401055943&amp;KeyName=labelbox-assets-key-3&amp;Signature=AP78M5-ygtSeOBLM6cifDTWKL6U</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F388a3201-70c0-2ad9-9d16-f1ae9c146436-20220423_143829.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=vS2gYjfdS2aBks0monWZnNyDgRs</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -1828,9 +1934,15 @@
         <v>155</v>
       </c>
       <c r="R18" t="n">
+        <v>912</v>
+      </c>
+      <c r="S18" t="n">
+        <v>2389</v>
+      </c>
+      <c r="T18" t="n">
         <v>0.7356828193832599</v>
       </c>
-      <c r="S18" t="n">
+      <c r="U18" t="n">
         <v>0.3018018018018018</v>
       </c>
     </row>
@@ -1890,7 +2002,7 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2fcaf846-c9d8-38e6-7159-93152bb7565d-20220423_143834.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=eYgJr8gMovgvnSAtuEKoyS8B67I</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2fcaf846-c9d8-38e6-7159-93152bb7565d-20220423_143834.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=dVKslkgLzX8GeFrass5vxlWmV_I</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
@@ -1905,9 +2017,15 @@
         <v>136</v>
       </c>
       <c r="R19" t="n">
+        <v>918</v>
+      </c>
+      <c r="S19" t="n">
+        <v>2386</v>
+      </c>
+      <c r="T19" t="n">
         <v>0.7533039647577092</v>
       </c>
-      <c r="S19" t="n">
+      <c r="U19" t="n">
         <v>0.3873873873873874</v>
       </c>
     </row>
@@ -1967,7 +2085,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F391640d3-8c0f-4480-32ff-849ded96f892-20220423_145106.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=OeCa9D0b__JfZ5LjsBByHG1_KkI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F391640d3-8c0f-4480-32ff-849ded96f892-20220423_145106.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=mxXd4LuUU9iob4KGWS2IKMCN3mo</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -1982,9 +2100,15 @@
         <v>196</v>
       </c>
       <c r="R20" t="n">
-        <v>0</v>
+        <v>752</v>
       </c>
       <c r="S20" t="n">
+        <v>2124</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2044,7 +2168,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb1c58ce7-d168-8ec2-c90e-d11353cf558a-20220423_145116.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=mpJDKsL5UEbDSo6QVyztnBR6blQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb1c58ce7-d168-8ec2-c90e-d11353cf558a-20220423_145116.jpg?Expires=1652726495783&amp;KeyName=labelbox-assets-key-3&amp;Signature=UHrTwnGyWMv056Sp7ze8EybWPUg</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -2059,9 +2183,15 @@
         <v>263</v>
       </c>
       <c r="R21" t="n">
+        <v>766</v>
+      </c>
+      <c r="S21" t="n">
+        <v>2044</v>
+      </c>
+      <c r="T21" t="n">
         <v>0.04885993485342022</v>
       </c>
-      <c r="S21" t="n">
+      <c r="U21" t="n">
         <v>-0.3418367346938775</v>
       </c>
     </row>
@@ -2121,7 +2251,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4336b0e1-bc99-a8ca-3bf1-46e9e5457de7-20220423_145124.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=4e4rs1oBhgpu-EadyUTRCu6NLo8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4336b0e1-bc99-a8ca-3bf1-46e9e5457de7-20220423_145124.jpg?Expires=1652726495784&amp;KeyName=labelbox-assets-key-3&amp;Signature=bzsZfiKNW672F4UzE2wH-5N536U</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -2136,9 +2266,15 @@
         <v>257</v>
       </c>
       <c r="R22" t="n">
+        <v>770</v>
+      </c>
+      <c r="S22" t="n">
+        <v>2076</v>
+      </c>
+      <c r="T22" t="n">
         <v>0.1596091205211726</v>
       </c>
-      <c r="S22" t="n">
+      <c r="U22" t="n">
         <v>-0.3112244897959184</v>
       </c>
     </row>
@@ -2198,7 +2334,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6aa2dbfb-261e-d19f-72b7-073484d15ac8-20220423_145129.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=p8rdDP_PXVcEizANG5jC-TXTRoo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6aa2dbfb-261e-d19f-72b7-073484d15ac8-20220423_145129.jpg?Expires=1652726495784&amp;KeyName=labelbox-assets-key-3&amp;Signature=xDJyxqr8cQW0sHrJlghBzDw8uEY</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -2213,9 +2349,15 @@
         <v>252</v>
       </c>
       <c r="R23" t="n">
+        <v>784</v>
+      </c>
+      <c r="S23" t="n">
+        <v>2078</v>
+      </c>
+      <c r="T23" t="n">
         <v>0.247557003257329</v>
       </c>
-      <c r="S23" t="n">
+      <c r="U23" t="n">
         <v>-0.2857142857142858</v>
       </c>
     </row>
@@ -2275,7 +2417,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6957b74b-ea14-dfaf-fb6d-ce39108b58b2-20220423_145134.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=wF7E3sUugH295g9hZmr462SyI2I</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6957b74b-ea14-dfaf-fb6d-ce39108b58b2-20220423_145134.jpg?Expires=1652726495784&amp;KeyName=labelbox-assets-key-3&amp;Signature=aV-E8cnlyoONm5jKbwHl-YvxKng</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
@@ -2290,9 +2432,15 @@
         <v>158</v>
       </c>
       <c r="R24" t="n">
+        <v>785</v>
+      </c>
+      <c r="S24" t="n">
+        <v>2076</v>
+      </c>
+      <c r="T24" t="n">
         <v>0.2703583061889251</v>
       </c>
-      <c r="S24" t="n">
+      <c r="U24" t="n">
         <v>0.1938775510204082</v>
       </c>
     </row>
@@ -2352,7 +2500,7 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0f53404f-622c-ce3a-e400-ac759f4a9aaa-20220423_145142.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=4VGYXI1Ud61by93NJ346AyozDGA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0f53404f-622c-ce3a-e400-ac759f4a9aaa-20220423_145142.jpg?Expires=1652726495784&amp;KeyName=labelbox-assets-key-3&amp;Signature=Aaetner-ID-uHExM5Fhc8iPAkSE</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
@@ -2367,9 +2515,15 @@
         <v>154</v>
       </c>
       <c r="R25" t="n">
+        <v>790</v>
+      </c>
+      <c r="S25" t="n">
+        <v>2074</v>
+      </c>
+      <c r="T25" t="n">
         <v>0.2638436482084691</v>
       </c>
-      <c r="S25" t="n">
+      <c r="U25" t="n">
         <v>0.2142857142857143</v>
       </c>
     </row>
@@ -2429,7 +2583,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc37bbf48-38d6-e827-c3e3-9ef684633479-20220423_145904.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=dVVH5kvVNZajKTGuuisDceCVZ-w</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc37bbf48-38d6-e827-c3e3-9ef684633479-20220423_145904.jpg?Expires=1652726495784&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ka_ZbZP313WaQdtTwzPB-q5fD2E</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -2444,9 +2598,15 @@
         <v>32</v>
       </c>
       <c r="R26" t="n">
-        <v>0</v>
+        <v>957</v>
       </c>
       <c r="S26" t="n">
+        <v>2221</v>
+      </c>
+      <c r="T26" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2506,7 +2666,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5e1fb35-c8d3-2b03-ed65-f1d51c2bedc3-20220423_145913.jpg?Expires=1652401055944&amp;KeyName=labelbox-assets-key-3&amp;Signature=RrC7I6WS_f5DskZfVKQOpKOkqbw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5e1fb35-c8d3-2b03-ed65-f1d51c2bedc3-20220423_145913.jpg?Expires=1652726495785&amp;KeyName=labelbox-assets-key-3&amp;Signature=hbJknOtW3RrWM4um9p3dOrWnagg</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -2521,9 +2681,15 @@
         <v>32</v>
       </c>
       <c r="R27" t="n">
+        <v>968</v>
+      </c>
+      <c r="S27" t="n">
+        <v>2215</v>
+      </c>
+      <c r="T27" t="n">
         <v>0.01986754966887416</v>
       </c>
-      <c r="S27" t="n">
+      <c r="U27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2583,7 +2749,7 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F72fbe587-c4d6-75cf-bc68-a55c6faeedac-20220423_145917.jpg?Expires=1652401055945&amp;KeyName=labelbox-assets-key-3&amp;Signature=ctm5l6nNSnTreBiwCtDjzu2rLSU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F72fbe587-c4d6-75cf-bc68-a55c6faeedac-20220423_145917.jpg?Expires=1652726495786&amp;KeyName=labelbox-assets-key-3&amp;Signature=jfQcz3tZ5oV2xPgSsodnGPmBsuQ</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
@@ -2598,9 +2764,15 @@
         <v>41</v>
       </c>
       <c r="R28" t="n">
+        <v>986</v>
+      </c>
+      <c r="S28" t="n">
+        <v>2198</v>
+      </c>
+      <c r="T28" t="n">
         <v>0.06953642384105962</v>
       </c>
-      <c r="S28" t="n">
+      <c r="U28" t="n">
         <v>-0.28125</v>
       </c>
     </row>
@@ -2660,7 +2832,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc8ca71f9-edac-3800-9f9c-39dc5371f2a3-20220423_145920.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=6w9fB-69CJlPkDrEI8UF83f9CKU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc8ca71f9-edac-3800-9f9c-39dc5371f2a3-20220423_145920.jpg?Expires=1652726495786&amp;KeyName=labelbox-assets-key-3&amp;Signature=dU8hOvWaYWoMe7D1lLnIPNvaV7c</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -2675,9 +2847,15 @@
         <v>38</v>
       </c>
       <c r="R29" t="n">
+        <v>989</v>
+      </c>
+      <c r="S29" t="n">
+        <v>2189</v>
+      </c>
+      <c r="T29" t="n">
         <v>0.1556291390728477</v>
       </c>
-      <c r="S29" t="n">
+      <c r="U29" t="n">
         <v>-0.1875</v>
       </c>
     </row>
@@ -2737,7 +2915,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F612cc526-32d4-4370-67e5-52c1c3b23f5e-20220423_145924.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=Jtmcrh4gwcfX_hCA58Xkhhy20GA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F612cc526-32d4-4370-67e5-52c1c3b23f5e-20220423_145924.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=SlNKn7C8iRmd5xRufhiEcEhWmIQ</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
@@ -2752,9 +2930,15 @@
         <v>20</v>
       </c>
       <c r="R30" t="n">
+        <v>1021</v>
+      </c>
+      <c r="S30" t="n">
+        <v>2195</v>
+      </c>
+      <c r="T30" t="n">
         <v>0.3774834437086093</v>
       </c>
-      <c r="S30" t="n">
+      <c r="U30" t="n">
         <v>0.375</v>
       </c>
     </row>
@@ -2814,7 +2998,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3b9910d1-9483-4472-fe6c-4208353ca81c-20220423_145929.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=t4niGrluUVseZsxeCh610KWL82g</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3b9910d1-9483-4472-fe6c-4208353ca81c-20220423_145929.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=KZ0JtzSkG9VcZWoRfK2TLoKha3g</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -2829,9 +3013,15 @@
         <v>18</v>
       </c>
       <c r="R31" t="n">
+        <v>1018</v>
+      </c>
+      <c r="S31" t="n">
+        <v>2180</v>
+      </c>
+      <c r="T31" t="n">
         <v>0.3774834437086093</v>
       </c>
-      <c r="S31" t="n">
+      <c r="U31" t="n">
         <v>0.4375</v>
       </c>
     </row>
@@ -2891,7 +3081,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F712dfefb-ca5c-25e0-6f34-7899210e120f-20220423_150315.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=V7kw1_H7O_w0Zy3Jkt7JIAwa1IY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F712dfefb-ca5c-25e0-6f34-7899210e120f-20220423_150315.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=nYlJhKuy7_d8CHT1PPVzow6SdbA</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
@@ -2906,9 +3096,15 @@
         <v>26</v>
       </c>
       <c r="R32" t="n">
-        <v>0</v>
+        <v>983</v>
       </c>
       <c r="S32" t="n">
+        <v>2204</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2968,7 +3164,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb8c776d2-a984-e987-ecc9-4e3c4c158920-20220423_150320.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=W-Iai2uTp8P4BhTCPOL2NJfuHh8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb8c776d2-a984-e987-ecc9-4e3c4c158920-20220423_150320.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=UQ8gMVpNCs6j4Ox1l_LeSSB10lc</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
@@ -2983,9 +3179,15 @@
         <v>29</v>
       </c>
       <c r="R33" t="n">
+        <v>999</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2201</v>
+      </c>
+      <c r="T33" t="n">
         <v>0.1276595744680851</v>
       </c>
-      <c r="S33" t="n">
+      <c r="U33" t="n">
         <v>-0.1153846153846154</v>
       </c>
     </row>
@@ -3045,7 +3247,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0fcac30d-6058-7cdb-5517-f59a97321207-20220423_150324.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=Vwcx83u1JDsC8-MUtoyj57_iO2c</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0fcac30d-6058-7cdb-5517-f59a97321207-20220423_150324.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=pi7NxuurMGA5WOi-dyykziM1Pds</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
@@ -3060,9 +3262,15 @@
         <v>30</v>
       </c>
       <c r="R34" t="n">
+        <v>953</v>
+      </c>
+      <c r="S34" t="n">
+        <v>2190</v>
+      </c>
+      <c r="T34" t="n">
         <v>-0.425531914893617</v>
       </c>
-      <c r="S34" t="n">
+      <c r="U34" t="n">
         <v>-0.1538461538461537</v>
       </c>
     </row>
@@ -3122,7 +3330,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F16145540-e2de-14c3-4452-aac713a9b136-20220423_150330.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=mCPSAnys1uFHQpyS0JVTw2eXw7o</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F16145540-e2de-14c3-4452-aac713a9b136-20220423_150330.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=RiNoSdPXfYyDqNhsfZ4pOUUMExg</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -3137,9 +3345,15 @@
         <v>26</v>
       </c>
       <c r="R35" t="n">
+        <v>941</v>
+      </c>
+      <c r="S35" t="n">
+        <v>2191</v>
+      </c>
+      <c r="T35" t="n">
         <v>-0.3723404255319149</v>
       </c>
-      <c r="S35" t="n">
+      <c r="U35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3199,7 +3413,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fadbf5484-e7a9-e57c-224e-9751236be1fe-20220423_150334.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=b0u7c8pSsnEUJJtEIFFG0PecgP8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fadbf5484-e7a9-e57c-224e-9751236be1fe-20220423_150334.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=JTPmaYVAbpqHcECdlnT3XlfUMVg</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
@@ -3214,9 +3428,15 @@
         <v>10</v>
       </c>
       <c r="R36" t="n">
+        <v>942</v>
+      </c>
+      <c r="S36" t="n">
+        <v>2197</v>
+      </c>
+      <c r="T36" t="n">
         <v>-0.4414893617021276</v>
       </c>
-      <c r="S36" t="n">
+      <c r="U36" t="n">
         <v>0.6153846153846154</v>
       </c>
     </row>
@@ -3276,7 +3496,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F32a932c1-f575-a023-26dd-d73d63ec4e2b-20220423_150341.jpg?Expires=1652401055946&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ts9bM25yabXj2SM17o15aDjQ7BA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F32a932c1-f575-a023-26dd-d73d63ec4e2b-20220423_150341.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=OQRqB3Zp8tzQ9tL28Vssr5WD67Y</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -3291,9 +3511,15 @@
         <v>4</v>
       </c>
       <c r="R37" t="n">
+        <v>938</v>
+      </c>
+      <c r="S37" t="n">
+        <v>2202</v>
+      </c>
+      <c r="T37" t="n">
         <v>-0.4627659574468086</v>
       </c>
-      <c r="S37" t="n">
+      <c r="U37" t="n">
         <v>0.8461538461538461</v>
       </c>
     </row>
@@ -3353,7 +3579,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3850978f-25f8-d478-06f8-c115bb7426ca-20220423_150744.jpg?Expires=1652401055947&amp;KeyName=labelbox-assets-key-3&amp;Signature=eY65oDKkB7LtFbbGJn9ym7GWUGs</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3850978f-25f8-d478-06f8-c115bb7426ca-20220423_150744.jpg?Expires=1652726495787&amp;KeyName=labelbox-assets-key-3&amp;Signature=qiLajV3BcP0BMoXJ6FaTwBk_puo</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -3368,9 +3594,15 @@
         <v>215</v>
       </c>
       <c r="R38" t="n">
-        <v>0</v>
+        <v>898</v>
       </c>
       <c r="S38" t="n">
+        <v>2300</v>
+      </c>
+      <c r="T38" t="n">
+        <v>0</v>
+      </c>
+      <c r="U38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3430,7 +3662,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1e59dcf0-d085-0016-eb05-f665a47efe77-20220423_150755.jpg?Expires=1652401055947&amp;KeyName=labelbox-assets-key-3&amp;Signature=6X3CLj3OXVtzDDaVh1Fu4A1J2Fg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1e59dcf0-d085-0016-eb05-f665a47efe77-20220423_150755.jpg?Expires=1652726495788&amp;KeyName=labelbox-assets-key-3&amp;Signature=B2NZctduERPDVOij-Rb3imq_RGg</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -3445,9 +3677,15 @@
         <v>284</v>
       </c>
       <c r="R39" t="n">
+        <v>950</v>
+      </c>
+      <c r="S39" t="n">
+        <v>2213</v>
+      </c>
+      <c r="T39" t="n">
         <v>0.3801369863013698</v>
       </c>
-      <c r="S39" t="n">
+      <c r="U39" t="n">
         <v>-0.3209302325581396</v>
       </c>
     </row>
@@ -3507,7 +3745,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F26e81768-a0be-12ad-c5f1-736c97dfa769-20220423_150759.jpg?Expires=1652401055947&amp;KeyName=labelbox-assets-key-3&amp;Signature=t6HOFgDQqKJnpgKNwJMdv8csMME</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F26e81768-a0be-12ad-c5f1-736c97dfa769-20220423_150759.jpg?Expires=1652726495788&amp;KeyName=labelbox-assets-key-3&amp;Signature=mpay-73bmJiFZGbD9KOtpvbqRjg</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
@@ -3522,9 +3760,15 @@
         <v>273</v>
       </c>
       <c r="R40" t="n">
+        <v>979</v>
+      </c>
+      <c r="S40" t="n">
+        <v>2196</v>
+      </c>
+      <c r="T40" t="n">
         <v>0.5924657534246576</v>
       </c>
-      <c r="S40" t="n">
+      <c r="U40" t="n">
         <v>-0.2697674418604652</v>
       </c>
     </row>
@@ -3584,7 +3828,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff361a7d9-851b-d804-cc4c-720af4e37300-20220423_150803.jpg?Expires=1652401055947&amp;KeyName=labelbox-assets-key-3&amp;Signature=2onJNtiqZaEUye1hXxiTiKNCXYk</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff361a7d9-851b-d804-cc4c-720af4e37300-20220423_150803.jpg?Expires=1652726495790&amp;KeyName=labelbox-assets-key-3&amp;Signature=VrLy5wQHlhG4OqM9-wimbdb98mQ</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
@@ -3599,9 +3843,15 @@
         <v>259</v>
       </c>
       <c r="R41" t="n">
+        <v>992</v>
+      </c>
+      <c r="S41" t="n">
+        <v>2192</v>
+      </c>
+      <c r="T41" t="n">
         <v>0.7226027397260274</v>
       </c>
-      <c r="S41" t="n">
+      <c r="U41" t="n">
         <v>-0.2046511627906977</v>
       </c>
     </row>
@@ -3661,7 +3911,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6ddf2ee6-a116-57c9-ec26-bd12a83243a3-20220423_150808.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=LllYuc-NylRIrT7C9-E1FOQhWdU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6ddf2ee6-a116-57c9-ec26-bd12a83243a3-20220423_150808.jpg?Expires=1652726495790&amp;KeyName=labelbox-assets-key-3&amp;Signature=VHVIeJveTjTPfvdn6__onRc8vBs</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
@@ -3676,9 +3926,15 @@
         <v>239</v>
       </c>
       <c r="R42" t="n">
+        <v>1005</v>
+      </c>
+      <c r="S42" t="n">
+        <v>2191</v>
+      </c>
+      <c r="T42" t="n">
         <v>0.8082191780821918</v>
       </c>
-      <c r="S42" t="n">
+      <c r="U42" t="n">
         <v>-0.1116279069767443</v>
       </c>
     </row>
@@ -3738,7 +3994,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7e97bb41-93f4-bd4b-51e7-201caa37937e-20220423_150814.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=Pw8zjKd-vQ3XjDi80iwEqzfoHCA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7e97bb41-93f4-bd4b-51e7-201caa37937e-20220423_150814.jpg?Expires=1652726495790&amp;KeyName=labelbox-assets-key-3&amp;Signature=YYf_Pw4jGvUfsdxr_K8KjHfa248</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
@@ -3753,9 +4009,15 @@
         <v>219</v>
       </c>
       <c r="R43" t="n">
+        <v>1009</v>
+      </c>
+      <c r="S43" t="n">
+        <v>2188</v>
+      </c>
+      <c r="T43" t="n">
         <v>0.8698630136986302</v>
       </c>
-      <c r="S43" t="n">
+      <c r="U43" t="n">
         <v>-0.01860465116279064</v>
       </c>
     </row>
@@ -3815,7 +4077,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F411abf79-8c89-46d1-3be3-4d95568d6d8b-20220423_151207.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=Aw197Idl19QJ9dvMI3zIpAS8NKY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F411abf79-8c89-46d1-3be3-4d95568d6d8b-20220423_151207.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=4pEJWDw21fyQwCTMtQmILpe0N8A</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
@@ -3830,9 +4092,15 @@
         <v>265</v>
       </c>
       <c r="R44" t="n">
-        <v>0</v>
+        <v>894</v>
       </c>
       <c r="S44" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3892,7 +4160,7 @@
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb72051cf-7493-9cfa-2097-39e873d8c0b6-20220423_151214.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=jupD4TmksuYS-JIK22v7s1t87GQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb72051cf-7493-9cfa-2097-39e873d8c0b6-20220423_151214.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=G09dWrfNq8LhCVOAVbNoGyCZPdA</t>
         </is>
       </c>
       <c r="O45" t="inlineStr">
@@ -3907,9 +4175,15 @@
         <v>254</v>
       </c>
       <c r="R45" t="n">
+        <v>951</v>
+      </c>
+      <c r="S45" t="n">
+        <v>2260</v>
+      </c>
+      <c r="T45" t="n">
         <v>0.3811320754716981</v>
       </c>
-      <c r="S45" t="n">
+      <c r="U45" t="n">
         <v>0.04150943396226414</v>
       </c>
     </row>
@@ -3969,7 +4243,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc44e61a2-ef69-5a90-a289-b5303bddbaf9-20220423_151219.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=cVknI2Y0AHX6ijy-EA60JNyTq2M</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc44e61a2-ef69-5a90-a289-b5303bddbaf9-20220423_151219.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=7EQiFjTTwASDkCDz75gTbK5FgrU</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
@@ -3984,9 +4258,15 @@
         <v>230</v>
       </c>
       <c r="R46" t="n">
+        <v>979</v>
+      </c>
+      <c r="S46" t="n">
+        <v>2258</v>
+      </c>
+      <c r="T46" t="n">
         <v>0.6037735849056604</v>
       </c>
-      <c r="S46" t="n">
+      <c r="U46" t="n">
         <v>0.1320754716981132</v>
       </c>
     </row>
@@ -4046,7 +4326,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F851a797d-1f41-306a-e162-8356d80436f3-20220423_151223.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=bPJAz_14VsZvqI8cgGQbvjN08IA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F851a797d-1f41-306a-e162-8356d80436f3-20220423_151223.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=nj_gM7NM2iUh5Op6zyNimsdsj2w</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
@@ -4061,9 +4341,15 @@
         <v>207</v>
       </c>
       <c r="R47" t="n">
+        <v>995</v>
+      </c>
+      <c r="S47" t="n">
+        <v>2259</v>
+      </c>
+      <c r="T47" t="n">
         <v>0.7358490566037736</v>
       </c>
-      <c r="S47" t="n">
+      <c r="U47" t="n">
         <v>0.2188679245283018</v>
       </c>
     </row>
@@ -4123,7 +4409,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6a9bdd25-9906-52f4-622e-8cbd1616f286-20220423_151228.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=hQPnRsWMFVTMvZD9g_bFsfleGZw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6a9bdd25-9906-52f4-622e-8cbd1616f286-20220423_151228.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=7J37E01pwXS5I3K3tez6rva-c-Q</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
@@ -4138,9 +4424,15 @@
         <v>190</v>
       </c>
       <c r="R48" t="n">
+        <v>1005</v>
+      </c>
+      <c r="S48" t="n">
+        <v>2256</v>
+      </c>
+      <c r="T48" t="n">
         <v>0.8226415094339623</v>
       </c>
-      <c r="S48" t="n">
+      <c r="U48" t="n">
         <v>0.2830188679245284</v>
       </c>
     </row>
@@ -4200,7 +4492,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fac393718-2af2-d751-c3a4-8eb0b8b22a34-20220423_151236.jpg?Expires=1652401055948&amp;KeyName=labelbox-assets-key-3&amp;Signature=7C92nkkwOJo8S7ihF3TgnSaz4fM</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fac393718-2af2-d751-c3a4-8eb0b8b22a34-20220423_151236.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=U8Mbi2OneOgd1-WWeMWe3tcp1Vo</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
@@ -4215,9 +4507,15 @@
         <v>167</v>
       </c>
       <c r="R49" t="n">
+        <v>1012</v>
+      </c>
+      <c r="S49" t="n">
+        <v>2260</v>
+      </c>
+      <c r="T49" t="n">
         <v>0.879245283018868</v>
       </c>
-      <c r="S49" t="n">
+      <c r="U49" t="n">
         <v>0.369811320754717</v>
       </c>
     </row>
@@ -4277,7 +4575,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F187e3bf4-edf5-583e-0fef-eebfc7230e4d-20220423_152357.jpg?Expires=1652401055949&amp;KeyName=labelbox-assets-key-3&amp;Signature=sU-DePpJhaJGIZLpJSzRhF6LZQ4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F187e3bf4-edf5-583e-0fef-eebfc7230e4d-20220423_152357.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=gcB3Aturdpc_m_uzFrZiA8_KkhI</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
@@ -4292,9 +4590,15 @@
         <v>312</v>
       </c>
       <c r="R50" t="n">
-        <v>0</v>
+        <v>914</v>
       </c>
       <c r="S50" t="n">
+        <v>2260</v>
+      </c>
+      <c r="T50" t="n">
+        <v>0</v>
+      </c>
+      <c r="U50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4354,7 +4658,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff63b9072-bdec-83a4-7f50-a84e0597830a-20220423_152405.jpg?Expires=1652401055949&amp;KeyName=labelbox-assets-key-3&amp;Signature=kjpGcoMaqnhN7hbpo-6z6Y5rli4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff63b9072-bdec-83a4-7f50-a84e0597830a-20220423_152405.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=Oa42YO_36O1eKEtMhrQgmVe1k3o</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
@@ -4369,9 +4673,15 @@
         <v>306</v>
       </c>
       <c r="R51" t="n">
+        <v>954</v>
+      </c>
+      <c r="S51" t="n">
+        <v>2267</v>
+      </c>
+      <c r="T51" t="n">
         <v>0.4743589743589743</v>
       </c>
-      <c r="S51" t="n">
+      <c r="U51" t="n">
         <v>0.01923076923076927</v>
       </c>
     </row>
@@ -4431,7 +4741,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd85def89-bbe1-8a19-5158-428157e3e87f-20220423_152410.jpg?Expires=1652401055949&amp;KeyName=labelbox-assets-key-3&amp;Signature=25hnSPBCRSiRBSZmXzFbLfjvtmY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd85def89-bbe1-8a19-5158-428157e3e87f-20220423_152410.jpg?Expires=1652726495791&amp;KeyName=labelbox-assets-key-3&amp;Signature=T3DwTTZxVYGp6XgMuP_bB2O9WoU</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
@@ -4446,9 +4756,15 @@
         <v>291</v>
       </c>
       <c r="R52" t="n">
+        <v>980</v>
+      </c>
+      <c r="S52" t="n">
+        <v>2266</v>
+      </c>
+      <c r="T52" t="n">
         <v>0.7094017094017093</v>
       </c>
-      <c r="S52" t="n">
+      <c r="U52" t="n">
         <v>0.06730769230769229</v>
       </c>
     </row>
@@ -4508,7 +4824,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4191393f-5a94-e653-710d-06cba2f47d8b-20220423_152427.jpg?Expires=1652401055949&amp;KeyName=labelbox-assets-key-3&amp;Signature=K6aWXTsLBSgBONseQ2GUfzYYndY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4191393f-5a94-e653-710d-06cba2f47d8b-20220423_152427.jpg?Expires=1652726495792&amp;KeyName=labelbox-assets-key-3&amp;Signature=RbA1YLNeQdMB5RYRZBCRS5aFGWo</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
@@ -4523,9 +4839,15 @@
         <v>270</v>
       </c>
       <c r="R53" t="n">
+        <v>995</v>
+      </c>
+      <c r="S53" t="n">
+        <v>2267</v>
+      </c>
+      <c r="T53" t="n">
         <v>0.8547008547008547</v>
       </c>
-      <c r="S53" t="n">
+      <c r="U53" t="n">
         <v>0.1346153846153846</v>
       </c>
     </row>
@@ -4585,7 +4907,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fabe27fc4-4663-9f21-77b1-3d22aa869c6e-20220423_152432.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=nkZJdDbUITwcsDFJbziiHp6cohU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fabe27fc4-4663-9f21-77b1-3d22aa869c6e-20220423_152432.jpg?Expires=1652726495792&amp;KeyName=labelbox-assets-key-3&amp;Signature=MYEtNa0GGe8rH6c8104RCqiXWYs</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
@@ -4600,9 +4922,15 @@
         <v>253</v>
       </c>
       <c r="R54" t="n">
+        <v>1003</v>
+      </c>
+      <c r="S54" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T54" t="n">
         <v>0.9316239316239316</v>
       </c>
-      <c r="S54" t="n">
+      <c r="U54" t="n">
         <v>0.1891025641025641</v>
       </c>
     </row>
@@ -4662,7 +4990,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F85a4c704-edbb-5b5e-fc0b-e69564cbd2e6-20220423_152437.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=VFoeYFXoFCaC86f6NnSFSFW1OfY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F85a4c704-edbb-5b5e-fc0b-e69564cbd2e6-20220423_152437.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=x3OEbZ_DuMgnCxi9LSmn7ja3DM0</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
@@ -4677,9 +5005,15 @@
         <v>237</v>
       </c>
       <c r="R55" t="n">
+        <v>1007</v>
+      </c>
+      <c r="S55" t="n">
+        <v>2266</v>
+      </c>
+      <c r="T55" t="n">
         <v>0.9871794871794872</v>
       </c>
-      <c r="S55" t="n">
+      <c r="U55" t="n">
         <v>0.2403846153846154</v>
       </c>
     </row>
@@ -4739,7 +5073,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe37bfec7-9137-6fb3-da94-a64d71a430a3-20220423_153138.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=llUpjscDzEJzMv1IACNWHaEPfC0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe37bfec7-9137-6fb3-da94-a64d71a430a3-20220423_153138.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=xjzu20zIyVYNAV8ECUh2je_fmvY</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
@@ -4754,9 +5088,15 @@
         <v>150</v>
       </c>
       <c r="R56" t="n">
-        <v>0</v>
+        <v>863</v>
       </c>
       <c r="S56" t="n">
+        <v>2334</v>
+      </c>
+      <c r="T56" t="n">
+        <v>0</v>
+      </c>
+      <c r="U56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4816,7 +5156,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc57f4db-1277-8027-04fa-33710a4b7359-20220423_153149.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=eBi7hGlR13qOn3KhN0ciuVprsyo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc57f4db-1277-8027-04fa-33710a4b7359-20220423_153149.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=9tc4pVvaq2UJ7GiPIRTe--vOI4E</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
@@ -4831,9 +5171,15 @@
         <v>205</v>
       </c>
       <c r="R57" t="n">
+        <v>944</v>
+      </c>
+      <c r="S57" t="n">
+        <v>2263</v>
+      </c>
+      <c r="T57" t="n">
         <v>0.4534883720930233</v>
       </c>
-      <c r="S57" t="n">
+      <c r="U57" t="n">
         <v>-0.3666666666666667</v>
       </c>
     </row>
@@ -4893,7 +5239,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe650325e-3243-4bf8-e9fa-417b820c61b2-20220423_153153.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=TBT2L5kMQy9Y7rLTocZ93aUB43c</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe650325e-3243-4bf8-e9fa-417b820c61b2-20220423_153153.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=no5ANRQjn-HLpF9vRqRJdarY42c</t>
         </is>
       </c>
       <c r="O58" t="inlineStr">
@@ -4908,9 +5254,15 @@
         <v>178</v>
       </c>
       <c r="R58" t="n">
+        <v>978</v>
+      </c>
+      <c r="S58" t="n">
+        <v>2261</v>
+      </c>
+      <c r="T58" t="n">
         <v>0.6337209302325582</v>
       </c>
-      <c r="S58" t="n">
+      <c r="U58" t="n">
         <v>-0.1866666666666668</v>
       </c>
     </row>
@@ -4970,7 +5322,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7cdc8d5b-220f-d43f-f0dc-eca37f797186-20220423_153207.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=TDTAxWiO_oFLXouOn3ctjyje5Co</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7cdc8d5b-220f-d43f-f0dc-eca37f797186-20220423_153207.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=PaaW9ApdXC4Jl756gpOQfSB-QRQ</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
@@ -4985,9 +5337,15 @@
         <v>182</v>
       </c>
       <c r="R59" t="n">
+        <v>1040</v>
+      </c>
+      <c r="S59" t="n">
+        <v>2261</v>
+      </c>
+      <c r="T59" t="n">
         <v>0.8837209302325582</v>
       </c>
-      <c r="S59" t="n">
+      <c r="U59" t="n">
         <v>-0.2133333333333334</v>
       </c>
     </row>
@@ -5047,7 +5405,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F95141d3e-00e4-25c3-f126-3172f8556628-20220423_153212.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=ER5DsOXqyW_6PNMjtLuwfDp_cuU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F95141d3e-00e4-25c3-f126-3172f8556628-20220423_153212.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=xhmEZTps8rEe4n3_yAZz9oz1KU4</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
@@ -5062,9 +5420,15 @@
         <v>163</v>
       </c>
       <c r="R60" t="n">
+        <v>1047</v>
+      </c>
+      <c r="S60" t="n">
+        <v>2262</v>
+      </c>
+      <c r="T60" t="n">
         <v>0.9418604651162791</v>
       </c>
-      <c r="S60" t="n">
+      <c r="U60" t="n">
         <v>-0.08666666666666667</v>
       </c>
     </row>
@@ -5124,7 +5488,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc9ea9218-f273-f64c-e48e-7c232924bfbb-20220423_153218.jpg?Expires=1652401055950&amp;KeyName=labelbox-assets-key-3&amp;Signature=HFy-oIv2RmGpfR6rw8jyi_efT0E</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc9ea9218-f273-f64c-e48e-7c232924bfbb-20220423_153218.jpg?Expires=1652726495793&amp;KeyName=labelbox-assets-key-3&amp;Signature=X9l03LdCSUQZvaUtqcfeqFutGdo</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
@@ -5139,9 +5503,15 @@
         <v>149</v>
       </c>
       <c r="R61" t="n">
+        <v>1053</v>
+      </c>
+      <c r="S61" t="n">
+        <v>2258</v>
+      </c>
+      <c r="T61" t="n">
         <v>0.9854651162790697</v>
       </c>
-      <c r="S61" t="n">
+      <c r="U61" t="n">
         <v>0.00666666666666671</v>
       </c>
     </row>
@@ -5201,7 +5571,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fee19e792-230e-9fa3-aea3-53cc7b7440fc-20220423_153412.jpg?Expires=1652401055951&amp;KeyName=labelbox-assets-key-3&amp;Signature=apJ5___iiTdnux12KP8nbrbNEk4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fee19e792-230e-9fa3-aea3-53cc7b7440fc-20220423_153412.jpg?Expires=1652726495794&amp;KeyName=labelbox-assets-key-3&amp;Signature=h1ojaAKS3PCzSQVnjsP-q-z0EOg</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
@@ -5216,9 +5586,15 @@
         <v>245</v>
       </c>
       <c r="R62" t="n">
-        <v>0</v>
+        <v>922</v>
       </c>
       <c r="S62" t="n">
+        <v>2260</v>
+      </c>
+      <c r="T62" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5278,7 +5654,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe2dc12b6-a818-bdbc-3345-c1a832d82501-20220423_153417.jpg?Expires=1652401055951&amp;KeyName=labelbox-assets-key-3&amp;Signature=t9_T8oYbeuyqx6cKz6DqOtXbovQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe2dc12b6-a818-bdbc-3345-c1a832d82501-20220423_153417.jpg?Expires=1652726495794&amp;KeyName=labelbox-assets-key-3&amp;Signature=55csKLCC_qYt1qcCnl3h85HoK2g</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
@@ -5293,9 +5669,15 @@
         <v>224</v>
       </c>
       <c r="R63" t="n">
+        <v>961</v>
+      </c>
+      <c r="S63" t="n">
+        <v>2262</v>
+      </c>
+      <c r="T63" t="n">
         <v>0.2408759124087592</v>
       </c>
-      <c r="S63" t="n">
+      <c r="U63" t="n">
         <v>0.08571428571428574</v>
       </c>
     </row>
@@ -5355,7 +5737,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa366c17-a88c-68a2-d906-7a4ac5ecf48e-20220423_153422.jpg?Expires=1652401055951&amp;KeyName=labelbox-assets-key-3&amp;Signature=5SNGXBQLsZerzi1vJ3S4DxYOWHI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa366c17-a88c-68a2-d906-7a4ac5ecf48e-20220423_153422.jpg?Expires=1652726495794&amp;KeyName=labelbox-assets-key-3&amp;Signature=UxkuHWp22rMmpqT3wxIy9rBj-RA</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
@@ -5370,9 +5752,15 @@
         <v>196</v>
       </c>
       <c r="R64" t="n">
+        <v>989</v>
+      </c>
+      <c r="S64" t="n">
+        <v>2261</v>
+      </c>
+      <c r="T64" t="n">
         <v>0.4343065693430657</v>
       </c>
-      <c r="S64" t="n">
+      <c r="U64" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -5432,7 +5820,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4f5f8c1d-e4f3-09c3-3cd0-fa3d727f7844-20220423_153426.jpg?Expires=1652401055951&amp;KeyName=labelbox-assets-key-3&amp;Signature=RhDNwzU85Rfx84XdJf-CZtTOsz4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4f5f8c1d-e4f3-09c3-3cd0-fa3d727f7844-20220423_153426.jpg?Expires=1652726495794&amp;KeyName=labelbox-assets-key-3&amp;Signature=mHHdz_Fp0EuuQvkRYjMAdDINjk8</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
@@ -5447,9 +5835,15 @@
         <v>172</v>
       </c>
       <c r="R65" t="n">
+        <v>1004</v>
+      </c>
+      <c r="S65" t="n">
+        <v>2262</v>
+      </c>
+      <c r="T65" t="n">
         <v>0.5547445255474452</v>
       </c>
-      <c r="S65" t="n">
+      <c r="U65" t="n">
         <v>0.2979591836734694</v>
       </c>
     </row>
@@ -5509,7 +5903,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb6cfe46d-de77-779d-4b98-831688d659e0-20220423_153430.jpg?Expires=1652401055951&amp;KeyName=labelbox-assets-key-3&amp;Signature=FJLXRIjIA6zJd96Ho-H5_LEWilw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb6cfe46d-de77-779d-4b98-831688d659e0-20220423_153430.jpg?Expires=1652726495794&amp;KeyName=labelbox-assets-key-3&amp;Signature=IRKNSuwFfw3wpdm118m34Ll8W3M</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
@@ -5524,9 +5918,15 @@
         <v>151</v>
       </c>
       <c r="R66" t="n">
+        <v>1014</v>
+      </c>
+      <c r="S66" t="n">
+        <v>2259</v>
+      </c>
+      <c r="T66" t="n">
         <v>0.6496350364963503</v>
       </c>
-      <c r="S66" t="n">
+      <c r="U66" t="n">
         <v>0.3836734693877552</v>
       </c>
     </row>
@@ -5586,7 +5986,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc0e82d54-f5a6-bb86-a5d1-62be5305e8ff-20220423_153434.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=jkhVJp-zxPL3teJjxyPu2MRz7ak</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc0e82d54-f5a6-bb86-a5d1-62be5305e8ff-20220423_153434.jpg?Expires=1652726495795&amp;KeyName=labelbox-assets-key-3&amp;Signature=nbNdetOXpmpHyAj6KLiYsBVEqeY</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
@@ -5601,9 +6001,15 @@
         <v>131</v>
       </c>
       <c r="R67" t="n">
+        <v>1026</v>
+      </c>
+      <c r="S67" t="n">
+        <v>2255</v>
+      </c>
+      <c r="T67" t="n">
         <v>0.7226277372262774</v>
       </c>
-      <c r="S67" t="n">
+      <c r="U67" t="n">
         <v>0.4653061224489796</v>
       </c>
     </row>
@@ -5663,7 +6069,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F28ba6856-100a-a7ec-8d42-7ab9fab866de-20220423_153847.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=a4hxdgGeIGiR-sTIadZ1k-Xhp0c</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F28ba6856-100a-a7ec-8d42-7ab9fab866de-20220423_153847.jpg?Expires=1652726495795&amp;KeyName=labelbox-assets-key-3&amp;Signature=Zy01gcGfTxlSr-qVzvLGTAmuhXs</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
@@ -5678,9 +6084,15 @@
         <v>317</v>
       </c>
       <c r="R68" t="n">
-        <v>0</v>
+        <v>952</v>
       </c>
       <c r="S68" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T68" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5740,7 +6152,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2c7ae321-3577-3a52-1a79-0a76d3ebb634-20220423_153857.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=WkEX6KmSnMjZ0b1d8H4qytzgeiY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2c7ae321-3577-3a52-1a79-0a76d3ebb634-20220423_153857.jpg?Expires=1652726495795&amp;KeyName=labelbox-assets-key-3&amp;Signature=H4qH1odYURtImY-hLI7j2NymkYU</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
@@ -5755,9 +6167,15 @@
         <v>306</v>
       </c>
       <c r="R69" t="n">
+        <v>1002</v>
+      </c>
+      <c r="S69" t="n">
+        <v>2266</v>
+      </c>
+      <c r="T69" t="n">
         <v>0.5779220779220779</v>
       </c>
-      <c r="S69" t="n">
+      <c r="U69" t="n">
         <v>0.03470031545741326</v>
       </c>
     </row>
@@ -5817,7 +6235,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7931b8d5-4b95-c779-012d-556c4b79b59e-20220423_153901.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=PdkflrEz5oKuhASOqdpPSCvZeDs</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7931b8d5-4b95-c779-012d-556c4b79b59e-20220423_153901.jpg?Expires=1652726495795&amp;KeyName=labelbox-assets-key-3&amp;Signature=ZohfulzAfk6cxFMgjsARRvT2apA</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
@@ -5832,9 +6250,15 @@
         <v>281</v>
       </c>
       <c r="R70" t="n">
+        <v>1027</v>
+      </c>
+      <c r="S70" t="n">
+        <v>2261</v>
+      </c>
+      <c r="T70" t="n">
         <v>0.8181818181818181</v>
       </c>
-      <c r="S70" t="n">
+      <c r="U70" t="n">
         <v>0.113564668769716</v>
       </c>
     </row>
@@ -5894,7 +6318,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe490c403-2cf5-b877-9eb9-3d86b93f341e-20220423_153904.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=md9rmRFpS8a7lfN1ZYGtWuQGBsE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe490c403-2cf5-b877-9eb9-3d86b93f341e-20220423_153904.jpg?Expires=1652726495795&amp;KeyName=labelbox-assets-key-3&amp;Signature=Pv5k6eKzIjidCiTfUHOGrFo5Wbc</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
@@ -5909,9 +6333,15 @@
         <v>257</v>
       </c>
       <c r="R71" t="n">
+        <v>1036</v>
+      </c>
+      <c r="S71" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T71" t="n">
         <v>0.961038961038961</v>
       </c>
-      <c r="S71" t="n">
+      <c r="U71" t="n">
         <v>0.1892744479495269</v>
       </c>
     </row>
@@ -5971,7 +6401,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F312f3fb5-1dae-d390-5249-f92c94324d5f-20220423_153908.jpg?Expires=1652401055952&amp;KeyName=labelbox-assets-key-3&amp;Signature=6n2Yw2VDYBTPFPeTGnelp7XvviM</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F312f3fb5-1dae-d390-5249-f92c94324d5f-20220423_153908.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=oMMbStPbR7Bq3f4H79PeX0GSG7U</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
@@ -5986,9 +6416,15 @@
         <v>239</v>
       </c>
       <c r="R72" t="n">
+        <v>1042</v>
+      </c>
+      <c r="S72" t="n">
+        <v>2271</v>
+      </c>
+      <c r="T72" t="n">
         <v>0.9935064935064936</v>
       </c>
-      <c r="S72" t="n">
+      <c r="U72" t="n">
         <v>0.2460567823343849</v>
       </c>
     </row>
@@ -6048,7 +6484,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6cc661d0-9307-830a-73f6-e41286bedad1-20220423_153912.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=hPv99W4zM7m-jkEziMxZC6O5Mk0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6cc661d0-9307-830a-73f6-e41286bedad1-20220423_153912.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=ONDzVZ_vpZKjI7bzBWGbQ002_cY</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
@@ -6063,9 +6499,15 @@
         <v>224</v>
       </c>
       <c r="R73" t="n">
+        <v>1041</v>
+      </c>
+      <c r="S73" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T73" t="n">
         <v>1</v>
       </c>
-      <c r="S73" t="n">
+      <c r="U73" t="n">
         <v>0.2933753943217665</v>
       </c>
     </row>
@@ -6125,7 +6567,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F89f00865-e062-0979-c9b8-304e9afa6f44-20220423_154155.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=BHBSOY2rnvZWd5fLh0O5hh1c1iY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F89f00865-e062-0979-c9b8-304e9afa6f44-20220423_154155.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=sVtoH_1_0lR-P3oebFbVMDCw6O8</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
@@ -6140,9 +6582,15 @@
         <v>240</v>
       </c>
       <c r="R74" t="n">
-        <v>0</v>
+        <v>861</v>
       </c>
       <c r="S74" t="n">
+        <v>2272</v>
+      </c>
+      <c r="T74" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6202,7 +6650,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F61ad6a27-04ff-36a6-40a5-d16b497cf95a-20220423_154200.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=4NbcO03BmomGCBRQ8cYmrt80-WA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F61ad6a27-04ff-36a6-40a5-d16b497cf95a-20220423_154200.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=LX-eDsrLS_nBmWTmvWAw7I5C4mc</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
@@ -6217,9 +6665,15 @@
         <v>233</v>
       </c>
       <c r="R75" t="n">
+        <v>889</v>
+      </c>
+      <c r="S75" t="n">
+        <v>2265</v>
+      </c>
+      <c r="T75" t="n">
         <v>0.1678571428571428</v>
       </c>
-      <c r="S75" t="n">
+      <c r="U75" t="n">
         <v>0.02916666666666667</v>
       </c>
     </row>
@@ -6279,7 +6733,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2d901a53-3e32-4f43-9883-6ee3f7d365b5-20220423_154203.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=Px-xUJqtDL1gAaKN5pv26_D2c7c</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2d901a53-3e32-4f43-9883-6ee3f7d365b5-20220423_154203.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=Z-Eghas4ujNtgsaRqFsox6I-_qs</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
@@ -6294,9 +6748,15 @@
         <v>202</v>
       </c>
       <c r="R76" t="n">
+        <v>923</v>
+      </c>
+      <c r="S76" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T76" t="n">
         <v>0.375</v>
       </c>
-      <c r="S76" t="n">
+      <c r="U76" t="n">
         <v>0.1583333333333333</v>
       </c>
     </row>
@@ -6356,7 +6816,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc7637f2-5ea1-8a38-d9db-923a30ec7c04-20220423_154207.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=KibDusQ1B7J6Iyt3VdRsm0hgss4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc7637f2-5ea1-8a38-d9db-923a30ec7c04-20220423_154207.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=FJe1m870BNVf-9Hu1TglaF4oNmk</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
@@ -6371,9 +6831,15 @@
         <v>177</v>
       </c>
       <c r="R77" t="n">
+        <v>942</v>
+      </c>
+      <c r="S77" t="n">
+        <v>2269</v>
+      </c>
+      <c r="T77" t="n">
         <v>0.5214285714285714</v>
       </c>
-      <c r="S77" t="n">
+      <c r="U77" t="n">
         <v>0.2625</v>
       </c>
     </row>
@@ -6433,7 +6899,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc1e89069-9600-b53d-d2db-295a32032806-20220423_154211.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=UXqZpVWa8EPbUwBOcxAzdGZ_Z2w</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc1e89069-9600-b53d-d2db-295a32032806-20220423_154211.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=eXKTX-0ekCcB7sBQmHV700er4nY</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
@@ -6448,9 +6914,15 @@
         <v>159</v>
       </c>
       <c r="R78" t="n">
+        <v>954</v>
+      </c>
+      <c r="S78" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T78" t="n">
         <v>0.6142857142857143</v>
       </c>
-      <c r="S78" t="n">
+      <c r="U78" t="n">
         <v>0.3375</v>
       </c>
     </row>
@@ -6510,7 +6982,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F636283aa-e771-bf5d-96d7-7fefd7819db8-20220423_154215.jpg?Expires=1652401055953&amp;KeyName=labelbox-assets-key-3&amp;Signature=XGFp0FUJqOHKCAoNn5z6NR_GXoU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F636283aa-e771-bf5d-96d7-7fefd7819db8-20220423_154215.jpg?Expires=1652726495796&amp;KeyName=labelbox-assets-key-3&amp;Signature=K-Wxaz85dkenS2ih-iiFVCsLhjM</t>
         </is>
       </c>
       <c r="O79" t="inlineStr">
@@ -6525,9 +6997,15 @@
         <v>139</v>
       </c>
       <c r="R79" t="n">
+        <v>962</v>
+      </c>
+      <c r="S79" t="n">
+        <v>2268</v>
+      </c>
+      <c r="T79" t="n">
         <v>0.6964285714285714</v>
       </c>
-      <c r="S79" t="n">
+      <c r="U79" t="n">
         <v>0.4208333333333333</v>
       </c>
     </row>
@@ -6587,7 +7065,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3d818c9-6efd-45cf-ff0f-df96c64cf96a-20220423_154440.jpg?Expires=1652401055954&amp;KeyName=labelbox-assets-key-3&amp;Signature=fWlq_SiXsxvtwYPYHtm2NBZJi4U</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3d818c9-6efd-45cf-ff0f-df96c64cf96a-20220423_154440.jpg?Expires=1652726495797&amp;KeyName=labelbox-assets-key-3&amp;Signature=rquCfvTHMVf2f-CyvsQfqW3J4Mg</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
@@ -6602,9 +7080,15 @@
         <v>246</v>
       </c>
       <c r="R80" t="n">
-        <v>0</v>
+        <v>851</v>
       </c>
       <c r="S80" t="n">
+        <v>2261</v>
+      </c>
+      <c r="T80" t="n">
+        <v>0</v>
+      </c>
+      <c r="U80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6664,7 +7148,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7ec688fb-4d4d-fb09-345a-f4f36496686f-20220423_154448.jpg?Expires=1652401055954&amp;KeyName=labelbox-assets-key-3&amp;Signature=_LSOJASLTqfkJIE4D-B3kTaTmQQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7ec688fb-4d4d-fb09-345a-f4f36496686f-20220423_154448.jpg?Expires=1652726495797&amp;KeyName=labelbox-assets-key-3&amp;Signature=QBy2VYFOkIMmG84DnREtvBZgFP8</t>
         </is>
       </c>
       <c r="O81" t="inlineStr">
@@ -6679,9 +7163,15 @@
         <v>222</v>
       </c>
       <c r="R81" t="n">
+        <v>865</v>
+      </c>
+      <c r="S81" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T81" t="n">
         <v>0.162962962962963</v>
       </c>
-      <c r="S81" t="n">
+      <c r="U81" t="n">
         <v>0.09756097560975607</v>
       </c>
     </row>
@@ -6741,7 +7231,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd3890844-112f-5deb-eb90-ff9b97bfde0f-20220423_154453.jpg?Expires=1652401055954&amp;KeyName=labelbox-assets-key-3&amp;Signature=E-MtRzdgeXIaykSsT-FCdXlgU9w</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd3890844-112f-5deb-eb90-ff9b97bfde0f-20220423_154453.jpg?Expires=1652726495797&amp;KeyName=labelbox-assets-key-3&amp;Signature=rUAgqcCpa1DtEtN2GjdJtZIAgms</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
@@ -6756,9 +7246,15 @@
         <v>195</v>
       </c>
       <c r="R82" t="n">
+        <v>895</v>
+      </c>
+      <c r="S82" t="n">
+        <v>2267</v>
+      </c>
+      <c r="T82" t="n">
         <v>0.3666666666666667</v>
       </c>
-      <c r="S82" t="n">
+      <c r="U82" t="n">
         <v>0.2073170731707317</v>
       </c>
     </row>
@@ -6818,7 +7314,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdfdeace5-7576-d32d-ea65-e7a35011a7f7-20220423_154458.jpg?Expires=1652401055954&amp;KeyName=labelbox-assets-key-3&amp;Signature=0QTIPHzANGIzjShncXByHEjfV0o</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdfdeace5-7576-d32d-ea65-e7a35011a7f7-20220423_154458.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=VzOXiEDO_XG50dRWkOtuAugqV-k</t>
         </is>
       </c>
       <c r="O83" t="inlineStr">
@@ -6833,9 +7329,15 @@
         <v>170</v>
       </c>
       <c r="R83" t="n">
+        <v>914</v>
+      </c>
+      <c r="S83" t="n">
+        <v>2266</v>
+      </c>
+      <c r="T83" t="n">
         <v>0.5037037037037038</v>
       </c>
-      <c r="S83" t="n">
+      <c r="U83" t="n">
         <v>0.3089430894308943</v>
       </c>
     </row>
@@ -6895,7 +7397,7 @@
       </c>
       <c r="N84" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9ca691fb-ea2a-c104-2e5f-358c84756821-20220423_154502.jpg?Expires=1652401055954&amp;KeyName=labelbox-assets-key-3&amp;Signature=mRPLzujNcvBJFYFz2IFkwbcOkVQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9ca691fb-ea2a-c104-2e5f-358c84756821-20220423_154502.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=PIbuUeHfvPJ5tqceoRP696FPIQE</t>
         </is>
       </c>
       <c r="O84" t="inlineStr">
@@ -6910,9 +7412,15 @@
         <v>147</v>
       </c>
       <c r="R84" t="n">
+        <v>930</v>
+      </c>
+      <c r="S84" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T84" t="n">
         <v>0.6074074074074074</v>
       </c>
-      <c r="S84" t="n">
+      <c r="U84" t="n">
         <v>0.4024390243902439</v>
       </c>
     </row>
@@ -6972,7 +7480,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F02d33f25-2815-f1b8-fedb-4225b25abcb2-20220423_154506.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=BULMdaF-5Jyjj13dTGw3cW_ZSIU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F02d33f25-2815-f1b8-fedb-4225b25abcb2-20220423_154506.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=FwoAcYslMRaUnSIOCZwTvCfyDcA</t>
         </is>
       </c>
       <c r="O85" t="inlineStr">
@@ -6987,9 +7495,15 @@
         <v>129</v>
       </c>
       <c r="R85" t="n">
+        <v>939</v>
+      </c>
+      <c r="S85" t="n">
+        <v>2265</v>
+      </c>
+      <c r="T85" t="n">
         <v>0.6703703703703704</v>
       </c>
-      <c r="S85" t="n">
+      <c r="U85" t="n">
         <v>0.475609756097561</v>
       </c>
     </row>
@@ -7049,7 +7563,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ffea45414-48ff-0c23-28fe-060d41ee8690-20220423_154928.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=5Z4JbbOtHnGGs8b_2b_C0o3Nh2E</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ffea45414-48ff-0c23-28fe-060d41ee8690-20220423_154928.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=cwefGkr-yGzr1SwN3CaIzp22p5Y</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
@@ -7064,9 +7578,15 @@
         <v>280</v>
       </c>
       <c r="R86" t="n">
-        <v>0</v>
+        <v>863</v>
       </c>
       <c r="S86" t="n">
+        <v>2274</v>
+      </c>
+      <c r="T86" t="n">
+        <v>0</v>
+      </c>
+      <c r="U86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7126,7 +7646,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fddb55817-0d75-d292-701c-58982422a039-20220423_154934.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=HHFePXC8MU8MZyi9UKLp1QzlNK4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fddb55817-0d75-d292-701c-58982422a039-20220423_154934.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=QVOtdUjshcHuulc3UsTl7KHnVjc</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
@@ -7141,9 +7661,15 @@
         <v>280</v>
       </c>
       <c r="R87" t="n">
+        <v>930</v>
+      </c>
+      <c r="S87" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T87" t="n">
         <v>0.4427480916030534</v>
       </c>
-      <c r="S87" t="n">
+      <c r="U87" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7203,7 +7729,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb3ec4677-6aeb-ef91-c4c9-921598f6890e-20220423_154939.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=az8XOabAPyORiYzyJwMuQ4v9EYY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb3ec4677-6aeb-ef91-c4c9-921598f6890e-20220423_154939.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=jO9C_y3c-G84JuWLbJgcQB6cMHg</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
@@ -7218,9 +7744,15 @@
         <v>251</v>
       </c>
       <c r="R88" t="n">
+        <v>961</v>
+      </c>
+      <c r="S88" t="n">
+        <v>2264</v>
+      </c>
+      <c r="T88" t="n">
         <v>0.6870229007633588</v>
       </c>
-      <c r="S88" t="n">
+      <c r="U88" t="n">
         <v>0.1035714285714285</v>
       </c>
     </row>
@@ -7280,7 +7812,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7df3fe6e-57ee-138e-04a1-90d4564c234e-20220423_154944.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=jlxTeBrhyPlPBvdWRfcO29NYso0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7df3fe6e-57ee-138e-04a1-90d4564c234e-20220423_154944.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=I5rLQ3hIdCj9zFIewTLtUDzSLNs</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
@@ -7295,9 +7827,15 @@
         <v>229</v>
       </c>
       <c r="R89" t="n">
+        <v>978</v>
+      </c>
+      <c r="S89" t="n">
+        <v>2266</v>
+      </c>
+      <c r="T89" t="n">
         <v>0.8015267175572519</v>
       </c>
-      <c r="S89" t="n">
+      <c r="U89" t="n">
         <v>0.1821428571428572</v>
       </c>
     </row>
@@ -7357,7 +7895,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F84d4559a-8252-16ad-c794-183bc5f77698-20220423_154948.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=Lr1uEC_Z5tlp61mlJ3LTgPEESaA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F84d4559a-8252-16ad-c794-183bc5f77698-20220423_154948.jpg?Expires=1652726495798&amp;KeyName=labelbox-assets-key-3&amp;Signature=q3VMPIcB_4Q7dlWqNkL6H7yOi7k</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
@@ -7372,9 +7910,15 @@
         <v>213</v>
       </c>
       <c r="R90" t="n">
+        <v>993</v>
+      </c>
+      <c r="S90" t="n">
+        <v>2265</v>
+      </c>
+      <c r="T90" t="n">
         <v>0.8931297709923665</v>
       </c>
-      <c r="S90" t="n">
+      <c r="U90" t="n">
         <v>0.2392857142857143</v>
       </c>
     </row>
@@ -7434,7 +7978,7 @@
       </c>
       <c r="N91" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8291a879-1db1-1d45-bf8c-a8c430829020-20220423_154953.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=m2qA5BJo9kLPWoQivYlCCsjRFf8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8291a879-1db1-1d45-bf8c-a8c430829020-20220423_154953.jpg?Expires=1652726495799&amp;KeyName=labelbox-assets-key-3&amp;Signature=sUleN8UyI2UhEPeVymuRM6fZcxs</t>
         </is>
       </c>
       <c r="O91" t="inlineStr">
@@ -7449,9 +7993,15 @@
         <v>199</v>
       </c>
       <c r="R91" t="n">
+        <v>1001</v>
+      </c>
+      <c r="S91" t="n">
+        <v>2263</v>
+      </c>
+      <c r="T91" t="n">
         <v>0.9580152671755725</v>
       </c>
-      <c r="S91" t="n">
+      <c r="U91" t="n">
         <v>0.2892857142857143</v>
       </c>
     </row>
@@ -7511,7 +8061,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcd03645d-f7fe-8254-adfa-3c81a720d532-20220423_161115.jpg?Expires=1652401055956&amp;KeyName=labelbox-assets-key-3&amp;Signature=qJo7HVLZuFepCzvchM5XVVl0mDc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcd03645d-f7fe-8254-adfa-3c81a720d532-20220423_161115.jpg?Expires=1652726495799&amp;KeyName=labelbox-assets-key-3&amp;Signature=Md5zhrmnRTPRExuAdsje6Z0WlKg</t>
         </is>
       </c>
       <c r="O92" t="inlineStr">
@@ -7526,9 +8076,15 @@
         <v>242</v>
       </c>
       <c r="R92" t="n">
-        <v>0</v>
+        <v>1213</v>
       </c>
       <c r="S92" t="n">
+        <v>2265</v>
+      </c>
+      <c r="T92" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7588,7 +8144,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2035e2c8-04c5-a1a0-d94f-11b545e055e0-20220423_161124.jpg?Expires=1652401055956&amp;KeyName=labelbox-assets-key-3&amp;Signature=xt9BUJKx0HxFZWrCQ2c1vl4TN1Q</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2035e2c8-04c5-a1a0-d94f-11b545e055e0-20220423_161124.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=H1ykIM_k-_tItaMoWXa8wwHuT8o</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
@@ -7603,9 +8159,15 @@
         <v>324</v>
       </c>
       <c r="R93" t="n">
+        <v>1263</v>
+      </c>
+      <c r="S93" t="n">
+        <v>2157</v>
+      </c>
+      <c r="T93" t="n">
         <v>0.648</v>
       </c>
-      <c r="S93" t="n">
+      <c r="U93" t="n">
         <v>-0.3388429752066116</v>
       </c>
     </row>
@@ -7665,7 +8227,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff0579b01-f358-2264-3da0-1b5ac1d67089-20220423_161129.jpg?Expires=1652401055956&amp;KeyName=labelbox-assets-key-3&amp;Signature=B7mYpY1IvweG8vlJF8RwGswLU4A</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff0579b01-f358-2264-3da0-1b5ac1d67089-20220423_161129.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ogns5TnvcMS1fyiGL3l3XDCLjSY</t>
         </is>
       </c>
       <c r="O94" t="inlineStr">
@@ -7680,9 +8242,15 @@
         <v>294</v>
       </c>
       <c r="R94" t="n">
+        <v>1284</v>
+      </c>
+      <c r="S94" t="n">
+        <v>2158</v>
+      </c>
+      <c r="T94" t="n">
         <v>0.792</v>
       </c>
-      <c r="S94" t="n">
+      <c r="U94" t="n">
         <v>-0.2148760330578512</v>
       </c>
     </row>
@@ -7742,7 +8310,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F20a4b0b7-7e38-b1a6-cd15-703564cf8653-20220423_161133.jpg?Expires=1652401055956&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ac0hOomcbwyHsurx3PemCB1ZWKE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F20a4b0b7-7e38-b1a6-cd15-703564cf8653-20220423_161133.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=FPFg9GNfLcd2bl_mT_1rT1o0odA</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -7757,9 +8325,15 @@
         <v>270</v>
       </c>
       <c r="R95" t="n">
+        <v>1319</v>
+      </c>
+      <c r="S95" t="n">
+        <v>2163</v>
+      </c>
+      <c r="T95" t="n">
         <v>0.9</v>
       </c>
-      <c r="S95" t="n">
+      <c r="U95" t="n">
         <v>-0.115702479338843</v>
       </c>
     </row>
@@ -7819,7 +8393,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe89237bb-58bc-a684-b75d-196f46b589ec-20220423_161139.jpg?Expires=1652401055955&amp;KeyName=labelbox-assets-key-3&amp;Signature=TpyzrgMpVGztW28HuxisdGvFUB0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe89237bb-58bc-a684-b75d-196f46b589ec-20220423_161139.jpg?Expires=1652726495799&amp;KeyName=labelbox-assets-key-3&amp;Signature=CLnkT4809X1UKS0CWmULPfylMRw</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -7834,9 +8408,15 @@
         <v>337</v>
       </c>
       <c r="R96" t="n">
+        <v>1332</v>
+      </c>
+      <c r="S96" t="n">
+        <v>2166</v>
+      </c>
+      <c r="T96" t="n">
         <v>0.968</v>
       </c>
-      <c r="S96" t="n">
+      <c r="U96" t="n">
         <v>-0.3925619834710743</v>
       </c>
     </row>
@@ -7896,7 +8476,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdc49532a-b326-c0b6-fd95-033959febddc-20220423_161143.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=wGsYMZLO_JLmArOsMRKa4ZWZ48Q</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fdc49532a-b326-c0b6-fd95-033959febddc-20220423_161143.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=_OMmYjuslMwXnGTgN-DoaZ73l8c</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -7911,9 +8491,15 @@
         <v>184</v>
       </c>
       <c r="R97" t="n">
+        <v>927</v>
+      </c>
+      <c r="S97" t="n">
+        <v>1686</v>
+      </c>
+      <c r="T97" t="n">
         <v>0.992</v>
       </c>
-      <c r="S97" t="n">
+      <c r="U97" t="n">
         <v>0.2396694214876033</v>
       </c>
     </row>
@@ -7973,7 +8559,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F55de0283-3fdd-71d6-6db8-9c407e4b0c3d-20220423_161757.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=8NqH9spOqwCe7unc35tyfg7rwDI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F55de0283-3fdd-71d6-6db8-9c407e4b0c3d-20220423_161757.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=cY8O0DlMO13D9mtw3rW63hAl1sI</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -7988,9 +8574,15 @@
         <v>270</v>
       </c>
       <c r="R98" t="n">
-        <v>0</v>
+        <v>768</v>
       </c>
       <c r="S98" t="n">
+        <v>1567</v>
+      </c>
+      <c r="T98" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8050,7 +8642,7 @@
       </c>
       <c r="N99" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0cb49a98-92b2-ccc1-496c-785e8a11eb9b-20220423_161802.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=VrWfrSPxL6Ey73QPEWdGG9k2Dl4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0cb49a98-92b2-ccc1-496c-785e8a11eb9b-20220423_161802.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=PhHOurjSZeUIzdzF2NzaXIrH63A</t>
         </is>
       </c>
       <c r="O99" t="inlineStr">
@@ -8065,9 +8657,15 @@
         <v>366</v>
       </c>
       <c r="R99" t="n">
+        <v>834</v>
+      </c>
+      <c r="S99" t="n">
+        <v>1508</v>
+      </c>
+      <c r="T99" t="n">
         <v>0.5991902834008097</v>
       </c>
-      <c r="S99" t="n">
+      <c r="U99" t="n">
         <v>-0.3555555555555556</v>
       </c>
     </row>
@@ -8127,7 +8725,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa136ee84-72c7-9266-7c5d-6c06c40537c9-20220423_161807.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=b7cU44gQzhATr9HHonb6EC2MYvg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa136ee84-72c7-9266-7c5d-6c06c40537c9-20220423_161807.jpg?Expires=1652726495800&amp;KeyName=labelbox-assets-key-3&amp;Signature=XDlhDeyk61LohZvgShXDLvcHWJE</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -8142,9 +8740,15 @@
         <v>335</v>
       </c>
       <c r="R100" t="n">
+        <v>873</v>
+      </c>
+      <c r="S100" t="n">
+        <v>1542</v>
+      </c>
+      <c r="T100" t="n">
         <v>0.8259109311740891</v>
       </c>
-      <c r="S100" t="n">
+      <c r="U100" t="n">
         <v>-0.2407407407407407</v>
       </c>
     </row>
@@ -8204,7 +8808,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff2f314b5-8412-d970-7ded-2d2acb12fa22-20220423_161811.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=YMp6fetJlMj7HBTt7KCeTy0JQP0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff2f314b5-8412-d970-7ded-2d2acb12fa22-20220423_161811.jpg?Expires=1652726495801&amp;KeyName=labelbox-assets-key-3&amp;Signature=pxWzxrqUWxJ7TVYR4Ug8DaQsbR8</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -8219,9 +8823,15 @@
         <v>314</v>
       </c>
       <c r="R101" t="n">
+        <v>886</v>
+      </c>
+      <c r="S101" t="n">
+        <v>1562</v>
+      </c>
+      <c r="T101" t="n">
         <v>0.9149797570850202</v>
       </c>
-      <c r="S101" t="n">
+      <c r="U101" t="n">
         <v>-0.162962962962963</v>
       </c>
     </row>
@@ -8281,7 +8891,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8dc7e370-45e3-f28a-6ffd-9fd68bfb41a3-20220423_161816.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=ohu66QUzGCW7rK5FMVTM-AZFoRA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8dc7e370-45e3-f28a-6ffd-9fd68bfb41a3-20220423_161816.jpg?Expires=1652726495801&amp;KeyName=labelbox-assets-key-3&amp;Signature=b4EbHfU3I71s9d4wPzve-O8C5DA</t>
         </is>
       </c>
       <c r="O102" t="inlineStr">
@@ -8296,9 +8906,15 @@
         <v>291</v>
       </c>
       <c r="R102" t="n">
+        <v>894</v>
+      </c>
+      <c r="S102" t="n">
+        <v>1579</v>
+      </c>
+      <c r="T102" t="n">
         <v>0.97165991902834</v>
       </c>
-      <c r="S102" t="n">
+      <c r="U102" t="n">
         <v>-0.07777777777777772</v>
       </c>
     </row>
@@ -8358,7 +8974,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F5233fb35-3ed3-6e40-e67b-f8f441393f76-20220423_161824.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=4nNsqxis_nSOQIAqMcy5d9arlyY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F5233fb35-3ed3-6e40-e67b-f8f441393f76-20220423_161824.jpg?Expires=1652726495801&amp;KeyName=labelbox-assets-key-3&amp;Signature=aJqXDmQRDMyiUkgumaX8IFrGVjU</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -8373,9 +8989,15 @@
         <v>274</v>
       </c>
       <c r="R103" t="n">
+        <v>902</v>
+      </c>
+      <c r="S103" t="n">
+        <v>1597</v>
+      </c>
+      <c r="T103" t="n">
         <v>0.9959514170040485</v>
       </c>
-      <c r="S103" t="n">
+      <c r="U103" t="n">
         <v>-0.01481481481481484</v>
       </c>
     </row>
@@ -8435,7 +9057,7 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F62e7dd66-7196-e0a7-0e86-fe7d4fbf70d8-20220423_162703.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=xX_9PCA-zZU1RrA3yNduluYbgRQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F62e7dd66-7196-e0a7-0e86-fe7d4fbf70d8-20220423_162703.jpg?Expires=1652726495801&amp;KeyName=labelbox-assets-key-3&amp;Signature=JGqyEbvfVsno2XSI6tcMbbH2mGg</t>
         </is>
       </c>
       <c r="O104" t="inlineStr">
@@ -8450,9 +9072,15 @@
         <v>321</v>
       </c>
       <c r="R104" t="n">
-        <v>0</v>
+        <v>768</v>
       </c>
       <c r="S104" t="n">
+        <v>1538</v>
+      </c>
+      <c r="T104" t="n">
+        <v>0</v>
+      </c>
+      <c r="U104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8512,7 +9140,7 @@
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2899fbf1-8f11-60d8-60ce-773a333cd3d2-20220423_162710.jpg?Expires=1652401055957&amp;KeyName=labelbox-assets-key-3&amp;Signature=DAdYqgqZbGC07YxhqGoybp8tyxA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2899fbf1-8f11-60d8-60ce-773a333cd3d2-20220423_162710.jpg?Expires=1652726495801&amp;KeyName=labelbox-assets-key-3&amp;Signature=i9SrcVdSi_6FcZvc4dV1DXm3lH4</t>
         </is>
       </c>
       <c r="O105" t="inlineStr">
@@ -8527,9 +9155,15 @@
         <v>311</v>
       </c>
       <c r="R105" t="n">
+        <v>848</v>
+      </c>
+      <c r="S105" t="n">
+        <v>1558</v>
+      </c>
+      <c r="T105" t="n">
         <v>0.5775193798449613</v>
       </c>
-      <c r="S105" t="n">
+      <c r="U105" t="n">
         <v>0.03115264797507789</v>
       </c>
     </row>
@@ -8589,7 +9223,7 @@
       </c>
       <c r="N106" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1cfde0ed-701c-e374-0e8b-5951814b14b9-20220423_162715.jpg?Expires=1652401055958&amp;KeyName=labelbox-assets-key-3&amp;Signature=QT__VLU_SsgKDFKxPJ2h34sq72o</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1cfde0ed-701c-e374-0e8b-5951814b14b9-20220423_162715.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=ujF8_fSaxc_IhOTtW10LO-_bai0</t>
         </is>
       </c>
       <c r="O106" t="inlineStr">
@@ -8604,9 +9238,15 @@
         <v>288</v>
       </c>
       <c r="R106" t="n">
+        <v>868</v>
+      </c>
+      <c r="S106" t="n">
+        <v>1587</v>
+      </c>
+      <c r="T106" t="n">
         <v>0.8720930232558139</v>
       </c>
-      <c r="S106" t="n">
+      <c r="U106" t="n">
         <v>0.102803738317757</v>
       </c>
     </row>
@@ -8666,7 +9306,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe86f3f2d-1553-ac5e-d765-5939f9394d6b-20220423_162720.jpg?Expires=1652401055958&amp;KeyName=labelbox-assets-key-3&amp;Signature=t9UHtyRl1lAc2qT3aIuNUqC3CIA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe86f3f2d-1553-ac5e-d765-5939f9394d6b-20220423_162720.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=ujjJJo-Gj_Jt_elyMAfKXMegQDM</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -8681,9 +9321,15 @@
         <v>261</v>
       </c>
       <c r="R107" t="n">
+        <v>847</v>
+      </c>
+      <c r="S107" t="n">
+        <v>1616</v>
+      </c>
+      <c r="T107" t="n">
         <v>0.9767441860465116</v>
       </c>
-      <c r="S107" t="n">
+      <c r="U107" t="n">
         <v>0.1869158878504673</v>
       </c>
     </row>
@@ -8743,7 +9389,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fbfd89923-93ba-6c5d-e9d6-f5c6f7d86c90-20220423_162726.jpg?Expires=1652401055958&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ib-HCS0KInRmarT30aJVDSCeEt8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fbfd89923-93ba-6c5d-e9d6-f5c6f7d86c90-20220423_162726.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=LGfhF8ymWRAP530BfOVRcKZc4NQ</t>
         </is>
       </c>
       <c r="O108" t="inlineStr">
@@ -8758,9 +9404,15 @@
         <v>235</v>
       </c>
       <c r="R108" t="n">
+        <v>818</v>
+      </c>
+      <c r="S108" t="n">
+        <v>1644</v>
+      </c>
+      <c r="T108" t="n">
         <v>0.9883720930232558</v>
       </c>
-      <c r="S108" t="n">
+      <c r="U108" t="n">
         <v>0.2679127725856698</v>
       </c>
     </row>
@@ -8820,7 +9472,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F06e58323-3ba3-2f2c-f194-957417e51db9-20220423_162734.jpg?Expires=1652401055958&amp;KeyName=labelbox-assets-key-3&amp;Signature=GSk7vfEjmpPVyP7qp5jVoRjKRM4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F06e58323-3ba3-2f2c-f194-957417e51db9-20220423_162734.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=hcCLSvNHFyZV9qdFH4tOZzgKv-0</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">
@@ -8835,9 +9487,15 @@
         <v>210</v>
       </c>
       <c r="R109" t="n">
+        <v>820</v>
+      </c>
+      <c r="S109" t="n">
+        <v>1671</v>
+      </c>
+      <c r="T109" t="n">
         <v>0.9883720930232558</v>
       </c>
-      <c r="S109" t="n">
+      <c r="U109" t="n">
         <v>0.3457943925233645</v>
       </c>
     </row>
@@ -8897,7 +9555,7 @@
       </c>
       <c r="N110" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F68d8afc4-c040-f5ff-1b74-f2eef56b73fa-20220423_164014.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=tZjF1adkH5mS-XOVlSmIEOr530E</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F68d8afc4-c040-f5ff-1b74-f2eef56b73fa-20220423_164014.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=qRDiYOXeVKVddH6XUVMZeR1M7yw</t>
         </is>
       </c>
       <c r="O110" t="inlineStr">
@@ -8912,9 +9570,15 @@
         <v>319</v>
       </c>
       <c r="R110" t="n">
-        <v>0</v>
+        <v>1120</v>
       </c>
       <c r="S110" t="n">
+        <v>1505</v>
+      </c>
+      <c r="T110" t="n">
+        <v>0</v>
+      </c>
+      <c r="U110" t="n">
         <v>0</v>
       </c>
     </row>
@@ -8974,7 +9638,7 @@
       </c>
       <c r="N111" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F030a884f-db8b-4f5c-148c-26bcca575c69-20220423_164023.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=TpdfulVLj-xwgezbV-qLYzbVTuc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F030a884f-db8b-4f5c-148c-26bcca575c69-20220423_164023.jpg?Expires=1652726495802&amp;KeyName=labelbox-assets-key-3&amp;Signature=ehwGe1dVVX9T5ebDB-2AvEKi5cc</t>
         </is>
       </c>
       <c r="O111" t="inlineStr">
@@ -8989,9 +9653,15 @@
         <v>339</v>
       </c>
       <c r="R111" t="n">
+        <v>1219</v>
+      </c>
+      <c r="S111" t="n">
+        <v>1538</v>
+      </c>
+      <c r="T111" t="n">
         <v>0.6890756302521008</v>
       </c>
-      <c r="S111" t="n">
+      <c r="U111" t="n">
         <v>-0.06269592476489039</v>
       </c>
     </row>
@@ -9051,7 +9721,7 @@
       </c>
       <c r="N112" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7f7b5484-d5bb-ac64-3b88-bc747a48b289-20220423_164028.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=218sq5A6Y998yKJLm05Ja1UOSVQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7f7b5484-d5bb-ac64-3b88-bc747a48b289-20220423_164028.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=FcK3GIQ_4Kkn_h_mJb5HyUq8HzU</t>
         </is>
       </c>
       <c r="O112" t="inlineStr">
@@ -9066,9 +9736,15 @@
         <v>303</v>
       </c>
       <c r="R112" t="n">
+        <v>1256</v>
+      </c>
+      <c r="S112" t="n">
+        <v>1574</v>
+      </c>
+      <c r="T112" t="n">
         <v>0.8907563025210083</v>
       </c>
-      <c r="S112" t="n">
+      <c r="U112" t="n">
         <v>0.05015673981191227</v>
       </c>
     </row>
@@ -9128,7 +9804,7 @@
       </c>
       <c r="N113" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F83f4c8c6-75e4-bc56-9fdb-df3b317bdd80-20220423_164033.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=daiPGexj2wz5wljxlKtmWenEJIg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F83f4c8c6-75e4-bc56-9fdb-df3b317bdd80-20220423_164033.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=neTho-oOfAsu-sSj4SK_6OTKVlU</t>
         </is>
       </c>
       <c r="O113" t="inlineStr">
@@ -9143,9 +9819,15 @@
         <v>304</v>
       </c>
       <c r="R113" t="n">
+        <v>1268</v>
+      </c>
+      <c r="S113" t="n">
+        <v>1567</v>
+      </c>
+      <c r="T113" t="n">
         <v>0.9789915966386554</v>
       </c>
-      <c r="S113" t="n">
+      <c r="U113" t="n">
         <v>0.04702194357366773</v>
       </c>
     </row>
@@ -9205,7 +9887,7 @@
       </c>
       <c r="N114" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa08c16e-e2a1-36f8-cfd2-55b42b3a148c-20220423_164038.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=HwWZG3ZtJZLVeqLFDgNQcablsRY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa08c16e-e2a1-36f8-cfd2-55b42b3a148c-20220423_164038.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=cj6k9YbYp0Gp8b4m01B3om4S-TU</t>
         </is>
       </c>
       <c r="O114" t="inlineStr">
@@ -9220,9 +9902,15 @@
         <v>299</v>
       </c>
       <c r="R114" t="n">
+        <v>1272</v>
+      </c>
+      <c r="S114" t="n">
+        <v>1574</v>
+      </c>
+      <c r="T114" t="n">
         <v>0.9915966386554622</v>
       </c>
-      <c r="S114" t="n">
+      <c r="U114" t="n">
         <v>0.06269592476489028</v>
       </c>
     </row>
@@ -9282,7 +9970,7 @@
       </c>
       <c r="N115" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2821a957-fa34-d0ef-be7b-2649a293b7af-20220423_164044.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=4xg_YgYG1NCuiZC_LRg53dLyAxQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F2821a957-fa34-d0ef-be7b-2649a293b7af-20220423_164044.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=-RYP6pfFZbm1MaqwMS1LD_o3DiM</t>
         </is>
       </c>
       <c r="O115" t="inlineStr">
@@ -9297,9 +9985,15 @@
         <v>288</v>
       </c>
       <c r="R115" t="n">
+        <v>1272</v>
+      </c>
+      <c r="S115" t="n">
+        <v>1583</v>
+      </c>
+      <c r="T115" t="n">
         <v>0.9873949579831933</v>
       </c>
-      <c r="S115" t="n">
+      <c r="U115" t="n">
         <v>0.09717868338557989</v>
       </c>
     </row>
@@ -9359,7 +10053,7 @@
       </c>
       <c r="N116" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa571d2d0-4a3b-1c3c-6e3c-246a6592c4dd-20220423_164432.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=c9O9BlsAi_lL08EvwoH9wEX8Ass</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa571d2d0-4a3b-1c3c-6e3c-246a6592c4dd-20220423_164432.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=v47V5Di9K_TWXE8E_lyGBi4GPjI</t>
         </is>
       </c>
       <c r="O116" t="inlineStr">
@@ -9374,9 +10068,15 @@
         <v>309</v>
       </c>
       <c r="R116" t="n">
-        <v>0</v>
+        <v>1132</v>
       </c>
       <c r="S116" t="n">
+        <v>1542</v>
+      </c>
+      <c r="T116" t="n">
+        <v>0</v>
+      </c>
+      <c r="U116" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9436,7 +10136,7 @@
       </c>
       <c r="N117" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F80529ba5-fbed-39c1-81a3-5c6087b16700-20220423_164442.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=C_oabVQHfkjs31WElAoNVKVYn1s</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F80529ba5-fbed-39c1-81a3-5c6087b16700-20220423_164442.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=6CX32jTOo7qWx3Pf30iGOZoevCA</t>
         </is>
       </c>
       <c r="O117" t="inlineStr">
@@ -9451,9 +10151,15 @@
         <v>306</v>
       </c>
       <c r="R117" t="n">
+        <v>1227</v>
+      </c>
+      <c r="S117" t="n">
+        <v>1576</v>
+      </c>
+      <c r="T117" t="n">
         <v>0.7543859649122807</v>
       </c>
-      <c r="S117" t="n">
+      <c r="U117" t="n">
         <v>0.009708737864077666</v>
       </c>
     </row>
@@ -9513,7 +10219,7 @@
       </c>
       <c r="N118" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F847c2730-44a0-a84f-a3f0-0a4c3f39f729-20220423_164446.jpg?Expires=1652401055959&amp;KeyName=labelbox-assets-key-3&amp;Signature=k6eFY4Isa0A72uBuo1crFx6D3Zc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F847c2730-44a0-a84f-a3f0-0a4c3f39f729-20220423_164446.jpg?Expires=1652726495803&amp;KeyName=labelbox-assets-key-3&amp;Signature=zhfbWBoNSibAiU5L9LPmydhl1tk</t>
         </is>
       </c>
       <c r="O118" t="inlineStr">
@@ -9528,9 +10234,15 @@
         <v>281</v>
       </c>
       <c r="R118" t="n">
+        <v>1242</v>
+      </c>
+      <c r="S118" t="n">
+        <v>1600</v>
+      </c>
+      <c r="T118" t="n">
         <v>0.9385964912280702</v>
       </c>
-      <c r="S118" t="n">
+      <c r="U118" t="n">
         <v>0.09061488673139162</v>
       </c>
     </row>
@@ -9590,7 +10302,7 @@
       </c>
       <c r="N119" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F302f35be-74bf-ea93-36f1-5b2678b19284-20220423_164450.jpg?Expires=1652401055960&amp;KeyName=labelbox-assets-key-3&amp;Signature=n2LWWwSBIIqQ8PFd5n_H0P9StRs</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F302f35be-74bf-ea93-36f1-5b2678b19284-20220423_164450.jpg?Expires=1652726495804&amp;KeyName=labelbox-assets-key-3&amp;Signature=v_PxY5zUGisGhYvil97EDolRvgI</t>
         </is>
       </c>
       <c r="O119" t="inlineStr">
@@ -9605,9 +10317,15 @@
         <v>262</v>
       </c>
       <c r="R119" t="n">
+        <v>1240</v>
+      </c>
+      <c r="S119" t="n">
+        <v>1619</v>
+      </c>
+      <c r="T119" t="n">
         <v>0.9692982456140351</v>
       </c>
-      <c r="S119" t="n">
+      <c r="U119" t="n">
         <v>0.1521035598705501</v>
       </c>
     </row>
@@ -9667,7 +10385,7 @@
       </c>
       <c r="N120" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc6648ebe-b47a-3441-1e0e-1de8e3b9e268-20220423_164455.jpg?Expires=1652401055960&amp;KeyName=labelbox-assets-key-3&amp;Signature=pSHvWwTeQ9Pq6L6eBnnM0xNEGFI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc6648ebe-b47a-3441-1e0e-1de8e3b9e268-20220423_164455.jpg?Expires=1652726495804&amp;KeyName=labelbox-assets-key-3&amp;Signature=YloIPT6xXC6-9pdUBpEt-qtzNWk</t>
         </is>
       </c>
       <c r="O120" t="inlineStr">
@@ -9682,9 +10400,15 @@
         <v>247</v>
       </c>
       <c r="R120" t="n">
+        <v>1246</v>
+      </c>
+      <c r="S120" t="n">
+        <v>1628</v>
+      </c>
+      <c r="T120" t="n">
         <v>0.9956140350877193</v>
       </c>
-      <c r="S120" t="n">
+      <c r="U120" t="n">
         <v>0.2006472491909385</v>
       </c>
     </row>
@@ -9744,7 +10468,7 @@
       </c>
       <c r="N121" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F77c21d64-3cd2-63af-888d-1f7616c602ca-20220423_164500.jpg?Expires=1652401055960&amp;KeyName=labelbox-assets-key-3&amp;Signature=6Cq49CdNJ-_b7Jy8pzK-TxmehBw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F77c21d64-3cd2-63af-888d-1f7616c602ca-20220423_164500.jpg?Expires=1652726495804&amp;KeyName=labelbox-assets-key-3&amp;Signature=D2WasPNew7g-EAKlJFqfWAQDIdw</t>
         </is>
       </c>
       <c r="O121" t="inlineStr">
@@ -9759,9 +10483,15 @@
         <v>294</v>
       </c>
       <c r="R121" t="n">
+        <v>1244</v>
+      </c>
+      <c r="S121" t="n">
+        <v>1590</v>
+      </c>
+      <c r="T121" t="n">
         <v>0.9956140350877193</v>
       </c>
-      <c r="S121" t="n">
+      <c r="U121" t="n">
         <v>0.04854368932038833</v>
       </c>
     </row>
@@ -9821,7 +10551,7 @@
       </c>
       <c r="N122" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa7426ad-2ba5-e85a-e196-f49cf2cc42a4-20220423_164749.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=OfWQLwaoMXIIi8Q3XJn_d7WzSZQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Faa7426ad-2ba5-e85a-e196-f49cf2cc42a4-20220423_164749.jpg?Expires=1652726495804&amp;KeyName=labelbox-assets-key-3&amp;Signature=xUg7NYWJ9ivDEZCdPNc2SK1EAuc</t>
         </is>
       </c>
       <c r="O122" t="inlineStr">
@@ -9836,9 +10566,15 @@
         <v>311</v>
       </c>
       <c r="R122" t="n">
-        <v>0</v>
+        <v>1159</v>
       </c>
       <c r="S122" t="n">
+        <v>1522</v>
+      </c>
+      <c r="T122" t="n">
+        <v>0</v>
+      </c>
+      <c r="U122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -9898,7 +10634,7 @@
       </c>
       <c r="N123" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7b93f253-c315-3f35-0ddc-23f1b8841006-20220423_164754.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=7KlVsHcYAaK45MnJc4KAG2_8TsQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7b93f253-c315-3f35-0ddc-23f1b8841006-20220423_164754.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=tzMLbCQgw14KX3KGTe4LAC9pRcw</t>
         </is>
       </c>
       <c r="O123" t="inlineStr">
@@ -9913,9 +10649,15 @@
         <v>333</v>
       </c>
       <c r="R123" t="n">
+        <v>1254</v>
+      </c>
+      <c r="S123" t="n">
+        <v>1548</v>
+      </c>
+      <c r="T123" t="n">
         <v>0.7489361702127659</v>
       </c>
-      <c r="S123" t="n">
+      <c r="U123" t="n">
         <v>-0.07073954983922826</v>
       </c>
     </row>
@@ -9975,7 +10717,7 @@
       </c>
       <c r="N124" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F957bd52b-5ae8-450e-d75a-5f6d356d2bcf-20220423_164759.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=TMwQZOn_MgaI5rUvdRFIvUcVCL4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F957bd52b-5ae8-450e-d75a-5f6d356d2bcf-20220423_164759.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=s_LWXx15JQIK_s06D0Yykztz3UY</t>
         </is>
       </c>
       <c r="O124" t="inlineStr">
@@ -9990,9 +10732,15 @@
         <v>291</v>
       </c>
       <c r="R124" t="n">
+        <v>1273</v>
+      </c>
+      <c r="S124" t="n">
+        <v>1579</v>
+      </c>
+      <c r="T124" t="n">
         <v>0.9872340425531915</v>
       </c>
-      <c r="S124" t="n">
+      <c r="U124" t="n">
         <v>0.06430868167202575</v>
       </c>
     </row>
@@ -10052,7 +10800,7 @@
       </c>
       <c r="N125" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe89a7445-61f7-282f-7783-b2fa6895564e-20220423_164803.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=fQSGbTXyPo64uU5pZUlH6XF3UZA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe89a7445-61f7-282f-7783-b2fa6895564e-20220423_164803.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=fpDurU0-__sjJfx_8BPvzEr9Ku4</t>
         </is>
       </c>
       <c r="O125" t="inlineStr">
@@ -10067,9 +10815,15 @@
         <v>276</v>
       </c>
       <c r="R125" t="n">
+        <v>1277</v>
+      </c>
+      <c r="S125" t="n">
+        <v>1597</v>
+      </c>
+      <c r="T125" t="n">
         <v>0.9957446808510638</v>
       </c>
-      <c r="S125" t="n">
+      <c r="U125" t="n">
         <v>0.112540192926045</v>
       </c>
     </row>
@@ -10129,7 +10883,7 @@
       </c>
       <c r="N126" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F71dfbb48-64c9-0861-55d4-472562311d99-20220423_164808.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=E79eN1BYnOQi1uIZgo6boPkSsgQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F71dfbb48-64c9-0861-55d4-472562311d99-20220423_164808.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=9mqL6DvjAbog6kBVeRmxNIsVFfQ</t>
         </is>
       </c>
       <c r="O126" t="inlineStr">
@@ -10144,9 +10898,15 @@
         <v>258</v>
       </c>
       <c r="R126" t="n">
+        <v>1275</v>
+      </c>
+      <c r="S126" t="n">
+        <v>1617</v>
+      </c>
+      <c r="T126" t="n">
         <v>0.9957446808510638</v>
       </c>
-      <c r="S126" t="n">
+      <c r="U126" t="n">
         <v>0.1704180064308681</v>
       </c>
     </row>
@@ -10206,7 +10966,7 @@
       </c>
       <c r="N127" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa9a05f80-d06b-e126-d2d7-0719c1197c25-20220423_164812.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=V6jZC6emb_POCEJRIm1FLJW8IWU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa9a05f80-d06b-e126-d2d7-0719c1197c25-20220423_164812.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=2r22EEtZfvyf0QvwBvZd9BDn5d8</t>
         </is>
       </c>
       <c r="O127" t="inlineStr">
@@ -10221,9 +10981,15 @@
         <v>233</v>
       </c>
       <c r="R127" t="n">
+        <v>1276</v>
+      </c>
+      <c r="S127" t="n">
+        <v>1633</v>
+      </c>
+      <c r="T127" t="n">
         <v>0.9957446808510638</v>
       </c>
-      <c r="S127" t="n">
+      <c r="U127" t="n">
         <v>0.2508038585209004</v>
       </c>
     </row>
@@ -10283,7 +11049,7 @@
       </c>
       <c r="N128" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa5a297cc-81b7-5c0e-f8bc-1d419d2b7e41-20220423_165244.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=621h4HOSAinoUnrK-TZOl0XCB6k</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa5a297cc-81b7-5c0e-f8bc-1d419d2b7e41-20220423_165244.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=xt1FsRQlurKah48r9zE26h9tPf8</t>
         </is>
       </c>
       <c r="O128" t="inlineStr">
@@ -10298,9 +11064,15 @@
         <v>267</v>
       </c>
       <c r="R128" t="n">
-        <v>0</v>
+        <v>1181</v>
       </c>
       <c r="S128" t="n">
+        <v>1480</v>
+      </c>
+      <c r="T128" t="n">
+        <v>0</v>
+      </c>
+      <c r="U128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10360,7 +11132,7 @@
       </c>
       <c r="N129" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff3817b61-28ac-d32b-5e4a-24e45313d42b-20220423_165251.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=SM8fNQehE8V_oER-KNAc18zkiek</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Ff3817b61-28ac-d32b-5e4a-24e45313d42b-20220423_165251.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=Oxfnu0DnBZWNXwKzBzL447eIsKY</t>
         </is>
       </c>
       <c r="O129" t="inlineStr">
@@ -10375,9 +11147,15 @@
         <v>298</v>
       </c>
       <c r="R129" t="n">
+        <v>1256</v>
+      </c>
+      <c r="S129" t="n">
+        <v>1509</v>
+      </c>
+      <c r="T129" t="n">
         <v>0.6129032258064516</v>
       </c>
-      <c r="S129" t="n">
+      <c r="U129" t="n">
         <v>-0.1161048689138577</v>
       </c>
     </row>
@@ -10437,7 +11215,7 @@
       </c>
       <c r="N130" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8076dcd2-383e-09fd-5d94-167744a2eebb-20220423_165255.jpg?Expires=1652401055961&amp;KeyName=labelbox-assets-key-3&amp;Signature=dxtsvnKr4aMv7RmCVFCVhwqRfFI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8076dcd2-383e-09fd-5d94-167744a2eebb-20220423_165255.jpg?Expires=1652726495805&amp;KeyName=labelbox-assets-key-3&amp;Signature=KsmTDNAtWVdoEY7RVOdJfTm6kl4</t>
         </is>
       </c>
       <c r="O130" t="inlineStr">
@@ -10452,9 +11230,15 @@
         <v>265</v>
       </c>
       <c r="R130" t="n">
+        <v>1278</v>
+      </c>
+      <c r="S130" t="n">
+        <v>1540</v>
+      </c>
+      <c r="T130" t="n">
         <v>0.7862903225806451</v>
       </c>
-      <c r="S130" t="n">
+      <c r="U130" t="n">
         <v>0.007490636704119868</v>
       </c>
     </row>
@@ -10514,7 +11298,7 @@
       </c>
       <c r="N131" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0cd91d57-c99b-0ef5-f14e-4822bb440337-20220423_165259.jpg?Expires=1652401055962&amp;KeyName=labelbox-assets-key-3&amp;Signature=kudnFSGtHfZZk-RhMpOOglL9IzM</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0cd91d57-c99b-0ef5-f14e-4822bb440337-20220423_165259.jpg?Expires=1652726495806&amp;KeyName=labelbox-assets-key-3&amp;Signature=Vm3h6ZuTKGNmFtmid84gX3AmoX8</t>
         </is>
       </c>
       <c r="O131" t="inlineStr">
@@ -10529,9 +11313,15 @@
         <v>238</v>
       </c>
       <c r="R131" t="n">
+        <v>1284</v>
+      </c>
+      <c r="S131" t="n">
+        <v>1563</v>
+      </c>
+      <c r="T131" t="n">
         <v>0.8709677419354839</v>
       </c>
-      <c r="S131" t="n">
+      <c r="U131" t="n">
         <v>0.1086142322097379</v>
       </c>
     </row>
@@ -10591,7 +11381,7 @@
       </c>
       <c r="N132" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F03ac4c63-8f06-03c4-04c9-46abbcc6dae7-20220423_165304.jpg?Expires=1652401055962&amp;KeyName=labelbox-assets-key-3&amp;Signature=RgJ9mHtlE_JuRO94fkLDESHLVK4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F03ac4c63-8f06-03c4-04c9-46abbcc6dae7-20220423_165304.jpg?Expires=1652726495806&amp;KeyName=labelbox-assets-key-3&amp;Signature=JsUt9xbe-AAUuOt3zdFP8FDsWm4</t>
         </is>
       </c>
       <c r="O132" t="inlineStr">
@@ -10606,9 +11396,15 @@
         <v>206</v>
       </c>
       <c r="R132" t="n">
+        <v>1295</v>
+      </c>
+      <c r="S132" t="n">
+        <v>1593</v>
+      </c>
+      <c r="T132" t="n">
         <v>0.9516129032258065</v>
       </c>
-      <c r="S132" t="n">
+      <c r="U132" t="n">
         <v>0.2284644194756554</v>
       </c>
     </row>
@@ -10668,7 +11464,7 @@
       </c>
       <c r="N133" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F31a1f263-8d08-741a-01d2-2d4a21356e54-20220423_165310.jpg?Expires=1652401055962&amp;KeyName=labelbox-assets-key-3&amp;Signature=DArwvubqBvtw5PLkhvOoxNMO7lA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F31a1f263-8d08-741a-01d2-2d4a21356e54-20220423_165310.jpg?Expires=1652726495806&amp;KeyName=labelbox-assets-key-3&amp;Signature=9xjpYTwv-PMl95rDmVJA0Ye-9UI</t>
         </is>
       </c>
       <c r="O133" t="inlineStr">
@@ -10683,9 +11479,15 @@
         <v>184</v>
       </c>
       <c r="R133" t="n">
+        <v>1299</v>
+      </c>
+      <c r="S133" t="n">
+        <v>1615</v>
+      </c>
+      <c r="T133" t="n">
         <v>0.9798387096774194</v>
       </c>
-      <c r="S133" t="n">
+      <c r="U133" t="n">
         <v>0.3108614232209738</v>
       </c>
     </row>
@@ -10745,7 +11547,7 @@
       </c>
       <c r="N134" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb6e9f6fa-a67a-f53a-4f20-322deadf827e-20220423_165610.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=HGM_S665O5xlV3b81-o23AO8RbA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb6e9f6fa-a67a-f53a-4f20-322deadf827e-20220423_165610.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=5ZE0TrhzKMozjd1D73RcGvXuULA</t>
         </is>
       </c>
       <c r="O134" t="inlineStr">
@@ -10760,9 +11562,15 @@
         <v>343</v>
       </c>
       <c r="R134" t="n">
-        <v>0</v>
+        <v>1240</v>
       </c>
       <c r="S134" t="n">
+        <v>1529</v>
+      </c>
+      <c r="T134" t="n">
+        <v>0</v>
+      </c>
+      <c r="U134" t="n">
         <v>0</v>
       </c>
     </row>
@@ -10822,7 +11630,7 @@
       </c>
       <c r="N135" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7e9deb93-bb31-34f7-6336-76afbff86bcb-20220423_165616.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=q6Gh32J3CdmuWp6aQujnWsiSmsE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7e9deb93-bb31-34f7-6336-76afbff86bcb-20220423_165616.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=-atvW-mopaPNgZS0AnPYDDwMXkc</t>
         </is>
       </c>
       <c r="O135" t="inlineStr">
@@ -10837,9 +11645,15 @@
         <v>362</v>
       </c>
       <c r="R135" t="n">
+        <v>1341</v>
+      </c>
+      <c r="S135" t="n">
+        <v>1550</v>
+      </c>
+      <c r="T135" t="n">
         <v>0.7121212121212122</v>
       </c>
-      <c r="S135" t="n">
+      <c r="U135" t="n">
         <v>-0.055393586005831</v>
       </c>
     </row>
@@ -10899,7 +11713,7 @@
       </c>
       <c r="N136" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcef22ac7-9fda-6049-481a-8d5d37fbbc6a-20220423_165621.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=sDywwGRqOXLyfZVcSZDfESIMYQw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcef22ac7-9fda-6049-481a-8d5d37fbbc6a-20220423_165621.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=-1ER4VZfF1Nq0S1SRMvprs8Oew0</t>
         </is>
       </c>
       <c r="O136" t="inlineStr">
@@ -10914,9 +11728,15 @@
         <v>319</v>
       </c>
       <c r="R136" t="n">
+        <v>1376</v>
+      </c>
+      <c r="S136" t="n">
+        <v>1589</v>
+      </c>
+      <c r="T136" t="n">
         <v>0.9318181818181819</v>
       </c>
-      <c r="S136" t="n">
+      <c r="U136" t="n">
         <v>0.06997084548104959</v>
       </c>
     </row>
@@ -10976,7 +11796,7 @@
       </c>
       <c r="N137" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb9da67f3-0a20-63a7-13dd-e3ecb4a64a56-20220423_165625.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=MT1M_6zuI2ep79znx8Zj1Spc3hE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb9da67f3-0a20-63a7-13dd-e3ecb4a64a56-20220423_165625.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=sBoZKB0j_NYtJ7b0YaAtytbkMgA</t>
         </is>
       </c>
       <c r="O137" t="inlineStr">
@@ -10991,9 +11811,15 @@
         <v>292</v>
       </c>
       <c r="R137" t="n">
+        <v>1383</v>
+      </c>
+      <c r="S137" t="n">
+        <v>1616</v>
+      </c>
+      <c r="T137" t="n">
         <v>0.9962121212121212</v>
       </c>
-      <c r="S137" t="n">
+      <c r="U137" t="n">
         <v>0.1486880466472303</v>
       </c>
     </row>
@@ -11053,7 +11879,7 @@
       </c>
       <c r="N138" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc57a806-6e6d-82db-b121-903f97d2dfde-20220423_165629.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=_MtAot9PvRW1JFy3m5_djaKu2ms</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fcc57a806-6e6d-82db-b121-903f97d2dfde-20220423_165629.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=39E7Q4sFzsaiP8rku95ed4tkTcA</t>
         </is>
       </c>
       <c r="O138" t="inlineStr">
@@ -11068,9 +11894,15 @@
         <v>267</v>
       </c>
       <c r="R138" t="n">
+        <v>1389</v>
+      </c>
+      <c r="S138" t="n">
+        <v>1638</v>
+      </c>
+      <c r="T138" t="n">
         <v>0.9962121212121212</v>
       </c>
-      <c r="S138" t="n">
+      <c r="U138" t="n">
         <v>0.2215743440233237</v>
       </c>
     </row>
@@ -11130,7 +11962,7 @@
       </c>
       <c r="N139" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1264da73-4660-f5ec-85c0-5f9ad97aa01f-20220423_165633.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=GL__xbRqvyYg1AYflViAd9sN-fo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1264da73-4660-f5ec-85c0-5f9ad97aa01f-20220423_165633.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=o3NtwoVP2WURB1kTMep1UTLY-6Q</t>
         </is>
       </c>
       <c r="O139" t="inlineStr">
@@ -11145,9 +11977,15 @@
         <v>247</v>
       </c>
       <c r="R139" t="n">
+        <v>1389</v>
+      </c>
+      <c r="S139" t="n">
+        <v>1661</v>
+      </c>
+      <c r="T139" t="n">
         <v>0.9962121212121212</v>
       </c>
-      <c r="S139" t="n">
+      <c r="U139" t="n">
         <v>0.2798833819241983</v>
       </c>
     </row>
@@ -11207,7 +12045,7 @@
       </c>
       <c r="N140" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9de27e49-f980-0655-66fa-6e9505705155-20220423_170129.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=PO_Ua8XYx5nLAVRP47oYYXdu_YU</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9de27e49-f980-0655-66fa-6e9505705155-20220423_170129.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=U4r-ixCS58Zk1D5JP3jlMsh9JBE</t>
         </is>
       </c>
       <c r="O140" t="inlineStr">
@@ -11222,9 +12060,15 @@
         <v>361</v>
       </c>
       <c r="R140" t="n">
-        <v>0</v>
+        <v>1150</v>
       </c>
       <c r="S140" t="n">
+        <v>1646</v>
+      </c>
+      <c r="T140" t="n">
+        <v>0</v>
+      </c>
+      <c r="U140" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11284,7 +12128,7 @@
       </c>
       <c r="N141" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0871f352-2f71-d004-5fb1-16a6d555018c-20220423_170139.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=Fd9YGK2pXfLusRPB5fa1hph18dg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0871f352-2f71-d004-5fb1-16a6d555018c-20220423_170139.jpg?Expires=1652726495807&amp;KeyName=labelbox-assets-key-3&amp;Signature=qbkg6ptQRo3ExKZF2TKMDTfziAk</t>
         </is>
       </c>
       <c r="O141" t="inlineStr">
@@ -11299,9 +12143,15 @@
         <v>373</v>
       </c>
       <c r="R141" t="n">
+        <v>1241</v>
+      </c>
+      <c r="S141" t="n">
+        <v>1673</v>
+      </c>
+      <c r="T141" t="n">
         <v>0.7233201581027668</v>
       </c>
-      <c r="S141" t="n">
+      <c r="U141" t="n">
         <v>-0.0332409972299168</v>
       </c>
     </row>
@@ -11361,7 +12211,7 @@
       </c>
       <c r="N142" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F21c4bf70-3f98-0754-3dac-cc7143758d7e-20220423_170144.jpg?Expires=1652401055963&amp;KeyName=labelbox-assets-key-3&amp;Signature=mOvJHOECSGoXb-pO4ponpsVkQL0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F21c4bf70-3f98-0754-3dac-cc7143758d7e-20220423_170144.jpg?Expires=1652726495808&amp;KeyName=labelbox-assets-key-3&amp;Signature=j1WOR7JNpRD8QLxu53lYPNQS5OQ</t>
         </is>
       </c>
       <c r="O142" t="inlineStr">
@@ -11376,9 +12226,15 @@
         <v>342</v>
       </c>
       <c r="R142" t="n">
+        <v>1261</v>
+      </c>
+      <c r="S142" t="n">
+        <v>1705</v>
+      </c>
+      <c r="T142" t="n">
         <v>0.8774703557312253</v>
       </c>
-      <c r="S142" t="n">
+      <c r="U142" t="n">
         <v>0.05263157894736847</v>
       </c>
     </row>
@@ -11438,7 +12294,7 @@
       </c>
       <c r="N143" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0b82f837-7c26-44f2-5554-9f7f80d5955e-20220423_170149.jpg?Expires=1652401055964&amp;KeyName=labelbox-assets-key-3&amp;Signature=zVmoal15511u3Sql7AYzS1KcF-U</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F0b82f837-7c26-44f2-5554-9f7f80d5955e-20220423_170149.jpg?Expires=1652726495808&amp;KeyName=labelbox-assets-key-3&amp;Signature=Y9I4CwNuF1rMQvI8Y_1R0H14VnI</t>
         </is>
       </c>
       <c r="O143" t="inlineStr">
@@ -11453,9 +12309,15 @@
         <v>317</v>
       </c>
       <c r="R143" t="n">
+        <v>1275</v>
+      </c>
+      <c r="S143" t="n">
+        <v>1728</v>
+      </c>
+      <c r="T143" t="n">
         <v>0.9762845849802372</v>
       </c>
-      <c r="S143" t="n">
+      <c r="U143" t="n">
         <v>0.1218836565096952</v>
       </c>
     </row>
@@ -11515,7 +12377,7 @@
       </c>
       <c r="N144" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8bf55427-7163-81ed-29f5-e713c00c7f8c-20220423_170154.jpg?Expires=1652401055964&amp;KeyName=labelbox-assets-key-3&amp;Signature=sLdhZfpTLvzNaUaVtGQIXQV7kjk</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8bf55427-7163-81ed-29f5-e713c00c7f8c-20220423_170154.jpg?Expires=1652726495808&amp;KeyName=labelbox-assets-key-3&amp;Signature=cTGXMkvEgwegZbnqaDG6XtBL1RM</t>
         </is>
       </c>
       <c r="O144" t="inlineStr">
@@ -11530,9 +12392,15 @@
         <v>297</v>
       </c>
       <c r="R144" t="n">
+        <v>1273</v>
+      </c>
+      <c r="S144" t="n">
+        <v>1755</v>
+      </c>
+      <c r="T144" t="n">
         <v>0.9960474308300395</v>
       </c>
-      <c r="S144" t="n">
+      <c r="U144" t="n">
         <v>0.1772853185595568</v>
       </c>
     </row>
@@ -11592,7 +12460,7 @@
       </c>
       <c r="N145" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc604480e-fbd4-45e2-17e7-de39288d409d-20220423_170209.jpg?Expires=1652401055965&amp;KeyName=labelbox-assets-key-3&amp;Signature=OTpBgReQs4mBrlWiQ9avwnob7MA</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc604480e-fbd4-45e2-17e7-de39288d409d-20220423_170209.jpg?Expires=1652726495809&amp;KeyName=labelbox-assets-key-3&amp;Signature=FjAvPEMrH5AyPnsnu2P1oRR0uYM</t>
         </is>
       </c>
       <c r="O145" t="inlineStr">
@@ -11607,9 +12475,15 @@
         <v>267</v>
       </c>
       <c r="R145" t="n">
+        <v>1274</v>
+      </c>
+      <c r="S145" t="n">
+        <v>1779</v>
+      </c>
+      <c r="T145" t="n">
         <v>0.9960474308300395</v>
       </c>
-      <c r="S145" t="n">
+      <c r="U145" t="n">
         <v>0.260387811634349</v>
       </c>
     </row>
@@ -11669,7 +12543,7 @@
       </c>
       <c r="N146" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F24864b2c-a889-795c-cfed-52b3badabbe0-20220423_170506.jpg?Expires=1652401055965&amp;KeyName=labelbox-assets-key-3&amp;Signature=X4H7H39-37XJnC3mCHSFfe2cGCo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F24864b2c-a889-795c-cfed-52b3badabbe0-20220423_170506.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=kCcLfvdsMJCrtqaZ4VPWJt3tX9I</t>
         </is>
       </c>
       <c r="O146" t="inlineStr">
@@ -11684,9 +12558,15 @@
         <v>345</v>
       </c>
       <c r="R146" t="n">
-        <v>0</v>
+        <v>1192</v>
       </c>
       <c r="S146" t="n">
+        <v>1666</v>
+      </c>
+      <c r="T146" t="n">
+        <v>0</v>
+      </c>
+      <c r="U146" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11746,7 +12626,7 @@
       </c>
       <c r="N147" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6c222c6e-dd54-5f0f-3343-b3f0080ea801-20220423_170511.jpg?Expires=1652401055965&amp;KeyName=labelbox-assets-key-3&amp;Signature=rC3kD25Elya5KmEvF6H6YQXsvC0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6c222c6e-dd54-5f0f-3343-b3f0080ea801-20220423_170511.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=E3PGGyiscnp90-T3Rp7wgcK-esU</t>
         </is>
       </c>
       <c r="O147" t="inlineStr">
@@ -11761,9 +12641,15 @@
         <v>355</v>
       </c>
       <c r="R147" t="n">
+        <v>1263</v>
+      </c>
+      <c r="S147" t="n">
+        <v>1690</v>
+      </c>
+      <c r="T147" t="n">
         <v>0.6186440677966102</v>
       </c>
-      <c r="S147" t="n">
+      <c r="U147" t="n">
         <v>-0.02898550724637672</v>
       </c>
     </row>
@@ -11823,7 +12709,7 @@
       </c>
       <c r="N148" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4ea2e361-abc5-6510-3aaa-6ffa5d073a07-20220423_170516.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=WVaiImpvRVBobRQz9V75VmDNNmc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F4ea2e361-abc5-6510-3aaa-6ffa5d073a07-20220423_170516.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=7m626GHMMU0J0UUdZ-uuHIA7BS4</t>
         </is>
       </c>
       <c r="O148" t="inlineStr">
@@ -11838,9 +12724,15 @@
         <v>336</v>
       </c>
       <c r="R148" t="n">
+        <v>1285</v>
+      </c>
+      <c r="S148" t="n">
+        <v>1725</v>
+      </c>
+      <c r="T148" t="n">
         <v>0.8389830508474576</v>
       </c>
-      <c r="S148" t="n">
+      <c r="U148" t="n">
         <v>0.02608695652173909</v>
       </c>
     </row>
@@ -11900,7 +12792,7 @@
       </c>
       <c r="N149" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36d59a6e-01f7-477f-13a8-5fca6dbf1826-20220423_170520.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=2yBAhtJCOEctAJSRiF29DlWhYrs</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36d59a6e-01f7-477f-13a8-5fca6dbf1826-20220423_170520.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=KmvxO-02a67HEkRh-EQvqNOv4SA</t>
         </is>
       </c>
       <c r="O149" t="inlineStr">
@@ -11915,9 +12807,15 @@
         <v>301</v>
       </c>
       <c r="R149" t="n">
+        <v>1292</v>
+      </c>
+      <c r="S149" t="n">
+        <v>1747</v>
+      </c>
+      <c r="T149" t="n">
         <v>0.9067796610169492</v>
       </c>
-      <c r="S149" t="n">
+      <c r="U149" t="n">
         <v>0.1275362318840579</v>
       </c>
     </row>
@@ -11977,7 +12875,7 @@
       </c>
       <c r="N150" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb5c5dfcf-4196-c6e6-7acd-8202c81f72ec-20220423_170525.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=2w0fXUMx5QS7qhYCrTvq61MD4TY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb5c5dfcf-4196-c6e6-7acd-8202c81f72ec-20220423_170525.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=9D3wV5GYGBD7DcxKeTYXNTVBSqI</t>
         </is>
       </c>
       <c r="O150" t="inlineStr">
@@ -11992,9 +12890,15 @@
         <v>270</v>
       </c>
       <c r="R150" t="n">
+        <v>1300</v>
+      </c>
+      <c r="S150" t="n">
+        <v>1771</v>
+      </c>
+      <c r="T150" t="n">
         <v>0.9830508474576272</v>
       </c>
-      <c r="S150" t="n">
+      <c r="U150" t="n">
         <v>0.2173913043478261</v>
       </c>
     </row>
@@ -12054,7 +12958,7 @@
       </c>
       <c r="N151" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7cec1fe3-6a3f-0561-ae3e-cf48153222cf-20220423_170530.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=FGA2UfpnwyKhFZDTL9wuk_P9pgY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F7cec1fe3-6a3f-0561-ae3e-cf48153222cf-20220423_170530.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=ERCCsGbgHy9n25IaqnJHQAoOV88</t>
         </is>
       </c>
       <c r="O151" t="inlineStr">
@@ -12069,9 +12973,15 @@
         <v>257</v>
       </c>
       <c r="R151" t="n">
+        <v>1304</v>
+      </c>
+      <c r="S151" t="n">
+        <v>1788</v>
+      </c>
+      <c r="T151" t="n">
         <v>0.9957627118644068</v>
       </c>
-      <c r="S151" t="n">
+      <c r="U151" t="n">
         <v>0.255072463768116</v>
       </c>
     </row>
@@ -12131,7 +13041,7 @@
       </c>
       <c r="N152" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3aca846-182b-9ce3-2619-f277bd849f60-20220423_170850.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=nFaIQOjjwDhkjSZzpl-B0yHg2oc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa3aca846-182b-9ce3-2619-f277bd849f60-20220423_170850.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=XGcvmnznh4a0GmVUeGwom0knChI</t>
         </is>
       </c>
       <c r="O152" t="inlineStr">
@@ -12146,9 +13056,15 @@
         <v>355</v>
       </c>
       <c r="R152" t="n">
-        <v>0</v>
+        <v>1299</v>
       </c>
       <c r="S152" t="n">
+        <v>1662</v>
+      </c>
+      <c r="T152" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12208,7 +13124,7 @@
       </c>
       <c r="N153" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6665a7af-7cf8-8f45-5bd2-445d5622597a-20220423_170858.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=vdZQVxz3lhDvc5_Evx7XJCCaVWI</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F6665a7af-7cf8-8f45-5bd2-445d5622597a-20220423_170858.jpg?Expires=1652726495810&amp;KeyName=labelbox-assets-key-3&amp;Signature=guCA9P2IwWWPB1D4Zw8CCEWw3ug</t>
         </is>
       </c>
       <c r="O153" t="inlineStr">
@@ -12223,9 +13139,15 @@
         <v>359</v>
       </c>
       <c r="R153" t="n">
+        <v>1367</v>
+      </c>
+      <c r="S153" t="n">
+        <v>1694</v>
+      </c>
+      <c r="T153" t="n">
         <v>0.5666666666666667</v>
       </c>
-      <c r="S153" t="n">
+      <c r="U153" t="n">
         <v>-0.0112676056338028</v>
       </c>
     </row>
@@ -12285,7 +13207,7 @@
       </c>
       <c r="N154" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36e496f2-17a5-7adc-6b41-858770af3bb6-20220423_170903.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=iANHYI374IFJuGLNnN31mPV6Pr8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36e496f2-17a5-7adc-6b41-858770af3bb6-20220423_170903.jpg?Expires=1652726495811&amp;KeyName=labelbox-assets-key-3&amp;Signature=DIuo22PDG1YaEmV2gNwTqYnqipc</t>
         </is>
       </c>
       <c r="O154" t="inlineStr">
@@ -12300,9 +13222,15 @@
         <v>333</v>
       </c>
       <c r="R154" t="n">
+        <v>1387</v>
+      </c>
+      <c r="S154" t="n">
+        <v>1721</v>
+      </c>
+      <c r="T154" t="n">
         <v>0.775</v>
       </c>
-      <c r="S154" t="n">
+      <c r="U154" t="n">
         <v>0.06197183098591552</v>
       </c>
     </row>
@@ -12362,7 +13290,7 @@
       </c>
       <c r="N155" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F53f891dd-bc3b-6a7a-0b24-b9998e2fd6d7-20220423_170906.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=9DugFlxP3xdFoQTy6hSYyk2pWC4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F53f891dd-bc3b-6a7a-0b24-b9998e2fd6d7-20220423_170906.jpg?Expires=1652726495811&amp;KeyName=labelbox-assets-key-3&amp;Signature=oTiGZffoZQBhuQZYKpguYvZrA_w</t>
         </is>
       </c>
       <c r="O155" t="inlineStr">
@@ -12377,9 +13305,15 @@
         <v>311</v>
       </c>
       <c r="R155" t="n">
+        <v>1398</v>
+      </c>
+      <c r="S155" t="n">
+        <v>1745</v>
+      </c>
+      <c r="T155" t="n">
         <v>0.8791666666666667</v>
       </c>
-      <c r="S155" t="n">
+      <c r="U155" t="n">
         <v>0.1239436619718309</v>
       </c>
     </row>
@@ -12439,7 +13373,7 @@
       </c>
       <c r="N156" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe8893546-525a-9db4-b33c-d1d5ae6d4e32-20220423_170911.jpg?Expires=1652401055966&amp;KeyName=labelbox-assets-key-3&amp;Signature=HzHVbuonU2rWNosXAq49PD0N43Q</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe8893546-525a-9db4-b33c-d1d5ae6d4e32-20220423_170911.jpg?Expires=1652726495811&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ye4ETca_oxM6C5AYAgkg5RnzOrM</t>
         </is>
       </c>
       <c r="O156" t="inlineStr">
@@ -12454,9 +13388,15 @@
         <v>287</v>
       </c>
       <c r="R156" t="n">
+        <v>1411</v>
+      </c>
+      <c r="S156" t="n">
+        <v>1767</v>
+      </c>
+      <c r="T156" t="n">
         <v>0.9666666666666667</v>
       </c>
-      <c r="S156" t="n">
+      <c r="U156" t="n">
         <v>0.1915492957746479</v>
       </c>
     </row>
@@ -12516,7 +13456,7 @@
       </c>
       <c r="N157" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1b2f7292-e9e5-2ef2-c773-77e6bbbebc46-20220423_170916.jpg?Expires=1652401055967&amp;KeyName=labelbox-assets-key-3&amp;Signature=gXArCXCSINUa0VDHPPDbsSoEnl0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F1b2f7292-e9e5-2ef2-c773-77e6bbbebc46-20220423_170916.jpg?Expires=1652726495811&amp;KeyName=labelbox-assets-key-3&amp;Signature=gxivXOmx_thC5TXF4ooU44ahxkk</t>
         </is>
       </c>
       <c r="O157" t="inlineStr">
@@ -12531,9 +13471,15 @@
         <v>271</v>
       </c>
       <c r="R157" t="n">
+        <v>1414</v>
+      </c>
+      <c r="S157" t="n">
+        <v>1786</v>
+      </c>
+      <c r="T157" t="n">
         <v>0.9958333333333333</v>
       </c>
-      <c r="S157" t="n">
+      <c r="U157" t="n">
         <v>0.2366197183098592</v>
       </c>
     </row>
@@ -12593,7 +13539,7 @@
       </c>
       <c r="N158" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe520c622-fb53-f0ca-5632-a6835da404b4-20220423_171223.jpg?Expires=1652401055967&amp;KeyName=labelbox-assets-key-3&amp;Signature=1HKsaCbdB5LZvrROylA_ZZ6cJTQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fe520c622-fb53-f0ca-5632-a6835da404b4-20220423_171223.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=BSH5PmBJljPZMVYrH0QzI5mq0b0</t>
         </is>
       </c>
       <c r="O158" t="inlineStr">
@@ -12608,9 +13554,15 @@
         <v>326</v>
       </c>
       <c r="R158" t="n">
-        <v>0</v>
+        <v>1288</v>
       </c>
       <c r="S158" t="n">
+        <v>1682</v>
+      </c>
+      <c r="T158" t="n">
+        <v>0</v>
+      </c>
+      <c r="U158" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12670,7 +13622,7 @@
       </c>
       <c r="N159" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F94560e1c-45cd-1d2f-7547-b566e5705a52-20220423_171227.jpg?Expires=1652401055967&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ay8kQc2_OANIp6-96LehT4XBMJM</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F94560e1c-45cd-1d2f-7547-b566e5705a52-20220423_171227.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=-3XIdQz4ZPG1QRpqH2H3koryCao</t>
         </is>
       </c>
       <c r="O159" t="inlineStr">
@@ -12685,9 +13637,15 @@
         <v>330</v>
       </c>
       <c r="R159" t="n">
+        <v>1312</v>
+      </c>
+      <c r="S159" t="n">
+        <v>1700</v>
+      </c>
+      <c r="T159" t="n">
         <v>0.3046875</v>
       </c>
-      <c r="S159" t="n">
+      <c r="U159" t="n">
         <v>-0.01226993865030668</v>
       </c>
     </row>
@@ -12747,7 +13705,7 @@
       </c>
       <c r="N160" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F10a0b7bb-8dcf-0d57-b5e5-b2378978d1a0-20220423_171232.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=bLVV17qmTv1i727zoaAVIAAkF0Q</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F10a0b7bb-8dcf-0d57-b5e5-b2378978d1a0-20220423_171232.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=p1cLFErtNIXbBCqke6-k5rxP7Ig</t>
         </is>
       </c>
       <c r="O160" t="inlineStr">
@@ -12762,9 +13720,15 @@
         <v>313</v>
       </c>
       <c r="R160" t="n">
+        <v>1370</v>
+      </c>
+      <c r="S160" t="n">
+        <v>1744</v>
+      </c>
+      <c r="T160" t="n">
         <v>0.6640625</v>
       </c>
-      <c r="S160" t="n">
+      <c r="U160" t="n">
         <v>0.03987730061349692</v>
       </c>
     </row>
@@ -12824,7 +13788,7 @@
       </c>
       <c r="N161" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa650951d-77ab-a6e4-951e-acb0934c35db-20220423_171238.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=Wxy1NEJQqtLI-4p8I9r25-DEPkE</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa650951d-77ab-a6e4-951e-acb0934c35db-20220423_171238.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=Z_YdXpGaxA3TQyJP5keKo5dQR9E</t>
         </is>
       </c>
       <c r="O161" t="inlineStr">
@@ -12839,9 +13803,15 @@
         <v>291</v>
       </c>
       <c r="R161" t="n">
+        <v>1405</v>
+      </c>
+      <c r="S161" t="n">
+        <v>1769</v>
+      </c>
+      <c r="T161" t="n">
         <v>0.8359375</v>
       </c>
-      <c r="S161" t="n">
+      <c r="U161" t="n">
         <v>0.1073619631901841</v>
       </c>
     </row>
@@ -12901,7 +13871,7 @@
       </c>
       <c r="N162" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F53063675-f44e-02f1-aa00-3083ebc3da3a-20220423_171243.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=Fcy9wJ9o_Y9nD3ayGR6ELZaF2Mo</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F53063675-f44e-02f1-aa00-3083ebc3da3a-20220423_171243.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=midnIZwKEX1B8vut5EOBrFzZPtY</t>
         </is>
       </c>
       <c r="O162" t="inlineStr">
@@ -12916,9 +13886,15 @@
         <v>274</v>
       </c>
       <c r="R162" t="n">
+        <v>1430</v>
+      </c>
+      <c r="S162" t="n">
+        <v>1786</v>
+      </c>
+      <c r="T162" t="n">
         <v>0.9609375</v>
       </c>
-      <c r="S162" t="n">
+      <c r="U162" t="n">
         <v>0.1595092024539877</v>
       </c>
     </row>
@@ -12978,7 +13954,7 @@
       </c>
       <c r="N163" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F736745ab-fc32-2bef-b544-d2ac1019e0e0-20220423_171249.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=Q4-lzRNPKsMCCrcKsLHtc7pie_k</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F736745ab-fc32-2bef-b544-d2ac1019e0e0-20220423_171249.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=FhpqnnEDE5F5oLAVOaXJPQ9zqHg</t>
         </is>
       </c>
       <c r="O163" t="inlineStr">
@@ -12993,9 +13969,15 @@
         <v>252</v>
       </c>
       <c r="R163" t="n">
+        <v>1432</v>
+      </c>
+      <c r="S163" t="n">
+        <v>1806</v>
+      </c>
+      <c r="T163" t="n">
         <v>0.99609375</v>
       </c>
-      <c r="S163" t="n">
+      <c r="U163" t="n">
         <v>0.2269938650306749</v>
       </c>
     </row>
@@ -13055,7 +14037,7 @@
       </c>
       <c r="N164" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fffeac1ac-5db1-58e3-50f9-5147b35180c9-20220423_171651.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=fp2Uylz-mvq95-NkUzFpR3fJsf8</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fffeac1ac-5db1-58e3-50f9-5147b35180c9-20220423_171651.jpg?Expires=1652726495812&amp;KeyName=labelbox-assets-key-3&amp;Signature=pddORpu_o4uAyABsvaNE_k9wr5c</t>
         </is>
       </c>
       <c r="O164" t="inlineStr">
@@ -13070,9 +14052,15 @@
         <v>128</v>
       </c>
       <c r="R164" t="n">
-        <v>0</v>
+        <v>1117</v>
       </c>
       <c r="S164" t="n">
+        <v>1811</v>
+      </c>
+      <c r="T164" t="n">
+        <v>0</v>
+      </c>
+      <c r="U164" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13132,7 +14120,7 @@
       </c>
       <c r="N165" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F900dedc1-6274-3f26-4f29-36cf28b36ec0-20220423_171658.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=IqoTkLUAFhdcw1acL6hn4eKl_l0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F900dedc1-6274-3f26-4f29-36cf28b36ec0-20220423_171658.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=Ic9fKPe3H6p91yqrx0EIHIj-vP4</t>
         </is>
       </c>
       <c r="O165" t="inlineStr">
@@ -13147,9 +14135,15 @@
         <v>396</v>
       </c>
       <c r="R165" t="n">
+        <v>1252</v>
+      </c>
+      <c r="S165" t="n">
+        <v>1652</v>
+      </c>
+      <c r="T165" t="n">
         <v>0.8333333333333334</v>
       </c>
-      <c r="S165" t="n">
+      <c r="U165" t="n">
         <v>-2.09375</v>
       </c>
     </row>
@@ -13209,7 +14203,7 @@
       </c>
       <c r="N166" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8fef57ec-7b04-c773-4331-bd901fb48bd6-20220423_171704.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=zjpVyNYYU-e3wfBczeG5RbYFCfg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8fef57ec-7b04-c773-4331-bd901fb48bd6-20220423_171704.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=3yJDLvrLGP9vAFW8OyBTiY9oNIE</t>
         </is>
       </c>
       <c r="O166" t="inlineStr">
@@ -13224,9 +14218,15 @@
         <v>362</v>
       </c>
       <c r="R166" t="n">
+        <v>1272</v>
+      </c>
+      <c r="S166" t="n">
+        <v>1687</v>
+      </c>
+      <c r="T166" t="n">
         <v>0.96</v>
       </c>
-      <c r="S166" t="n">
+      <c r="U166" t="n">
         <v>-1.828125</v>
       </c>
     </row>
@@ -13286,7 +14286,7 @@
       </c>
       <c r="N167" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8571bb4e-ec87-c97f-7356-fabdc29d513f-20220423_171707.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=jt9yboA4HE3Hl0HCyzIUaxmHBoY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F8571bb4e-ec87-c97f-7356-fabdc29d513f-20220423_171707.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=1DQrCjii2Lim8olY7yRTmA0bc1o</t>
         </is>
       </c>
       <c r="O167" t="inlineStr">
@@ -13301,9 +14301,15 @@
         <v>343</v>
       </c>
       <c r="R167" t="n">
+        <v>1276</v>
+      </c>
+      <c r="S167" t="n">
+        <v>1711</v>
+      </c>
+      <c r="T167" t="n">
         <v>0.9966666666666667</v>
       </c>
-      <c r="S167" t="n">
+      <c r="U167" t="n">
         <v>-1.6796875</v>
       </c>
     </row>
@@ -13363,7 +14369,7 @@
       </c>
       <c r="N168" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F54e552ad-6f8c-9368-ba52-404051c8da1a-20220423_171712.jpg?Expires=1652401055968&amp;KeyName=labelbox-assets-key-3&amp;Signature=ir5s2jl1Q_bYN7DSeE6XCjYafRs</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F54e552ad-6f8c-9368-ba52-404051c8da1a-20220423_171712.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=8Nr-b2-H6-9_lTWFIqcwiszk9uk</t>
         </is>
       </c>
       <c r="O168" t="inlineStr">
@@ -13378,9 +14384,15 @@
         <v>313</v>
       </c>
       <c r="R168" t="n">
+        <v>1270</v>
+      </c>
+      <c r="S168" t="n">
+        <v>1734</v>
+      </c>
+      <c r="T168" t="n">
         <v>0.9966666666666667</v>
       </c>
-      <c r="S168" t="n">
+      <c r="U168" t="n">
         <v>-1.4453125</v>
       </c>
     </row>
@@ -13440,7 +14452,7 @@
       </c>
       <c r="N169" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Feb8deaca-3c2b-4c75-accd-7efe7bb10039-20220423_171717.jpg?Expires=1652401055969&amp;KeyName=labelbox-assets-key-3&amp;Signature=GvRHib4tHMx5-YVeLkwd81NJnes</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Feb8deaca-3c2b-4c75-accd-7efe7bb10039-20220423_171717.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=JDquI2vtEckXpqg8S65bGpRrL04</t>
         </is>
       </c>
       <c r="O169" t="inlineStr">
@@ -13455,9 +14467,15 @@
         <v>295</v>
       </c>
       <c r="R169" t="n">
+        <v>1274</v>
+      </c>
+      <c r="S169" t="n">
+        <v>1756</v>
+      </c>
+      <c r="T169" t="n">
         <v>0.9966666666666667</v>
       </c>
-      <c r="S169" t="n">
+      <c r="U169" t="n">
         <v>-1.3046875</v>
       </c>
     </row>
@@ -13517,7 +14535,7 @@
       </c>
       <c r="N170" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc6459609-3dab-20d5-4264-2ffb7b998d74-20220423_172107.jpg?Expires=1652401055969&amp;KeyName=labelbox-assets-key-3&amp;Signature=BVwnln8IeN8zMw2fmDXLv8uodQQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fc6459609-3dab-20d5-4264-2ffb7b998d74-20220423_172107.jpg?Expires=1652726495813&amp;KeyName=labelbox-assets-key-3&amp;Signature=ra2hpC0zmVjaq2vI3BTQ3xfbdKs</t>
         </is>
       </c>
       <c r="O170" t="inlineStr">
@@ -13532,9 +14550,15 @@
         <v>348</v>
       </c>
       <c r="R170" t="n">
-        <v>0</v>
+        <v>1187</v>
       </c>
       <c r="S170" t="n">
+        <v>1661</v>
+      </c>
+      <c r="T170" t="n">
+        <v>0</v>
+      </c>
+      <c r="U170" t="n">
         <v>0</v>
       </c>
     </row>
@@ -13594,7 +14618,7 @@
       </c>
       <c r="N171" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36de3080-2cbb-c24b-3aec-3224ea94f959-20220423_172114.jpg?Expires=1652401055969&amp;KeyName=labelbox-assets-key-3&amp;Signature=x3oBgfoECWjb2W_MFRl5E43-eZw</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F36de3080-2cbb-c24b-3aec-3224ea94f959-20220423_172114.jpg?Expires=1652726495814&amp;KeyName=labelbox-assets-key-3&amp;Signature=JJ4OS_8y1NShHM9iGGRYR3Bz8JM</t>
         </is>
       </c>
       <c r="O171" t="inlineStr">
@@ -13609,9 +14633,15 @@
         <v>394</v>
       </c>
       <c r="R171" t="n">
+        <v>1251</v>
+      </c>
+      <c r="S171" t="n">
+        <v>1656</v>
+      </c>
+      <c r="T171" t="n">
         <v>0.535031847133758</v>
       </c>
-      <c r="S171" t="n">
+      <c r="U171" t="n">
         <v>-0.132183908045977</v>
       </c>
     </row>
@@ -13671,7 +14701,7 @@
       </c>
       <c r="N172" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F712a1331-8310-3e94-9b94-99731e3305b3-20220423_172118.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=qM7f7GbiUtxbeHxu6szYJcI-L08</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F712a1331-8310-3e94-9b94-99731e3305b3-20220423_172118.jpg?Expires=1652726495814&amp;KeyName=labelbox-assets-key-3&amp;Signature=7LPQGdUrgAy6sh7K1Niw3VVqgwA</t>
         </is>
       </c>
       <c r="O172" t="inlineStr">
@@ -13686,9 +14716,15 @@
         <v>356</v>
       </c>
       <c r="R172" t="n">
+        <v>1293</v>
+      </c>
+      <c r="S172" t="n">
+        <v>1697</v>
+      </c>
+      <c r="T172" t="n">
         <v>0.7961783439490446</v>
       </c>
-      <c r="S172" t="n">
+      <c r="U172" t="n">
         <v>-0.02298850574712641</v>
       </c>
     </row>
@@ -13748,7 +14784,7 @@
       </c>
       <c r="N173" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F55f19f35-e412-9cf1-fa36-9bd217b9fd22-20220423_172122.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=Z8Yn2f2D8PEGUgujclR7ihJzPVg</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F55f19f35-e412-9cf1-fa36-9bd217b9fd22-20220423_172122.jpg?Expires=1652726495814&amp;KeyName=labelbox-assets-key-3&amp;Signature=byKccQ9r-qDeIhGkdoRKATpA8dE</t>
         </is>
       </c>
       <c r="O173" t="inlineStr">
@@ -13763,9 +14799,15 @@
         <v>333</v>
       </c>
       <c r="R173" t="n">
+        <v>1302</v>
+      </c>
+      <c r="S173" t="n">
+        <v>1722</v>
+      </c>
+      <c r="T173" t="n">
         <v>0.8757961783439491</v>
       </c>
-      <c r="S173" t="n">
+      <c r="U173" t="n">
         <v>0.0431034482758621</v>
       </c>
     </row>
@@ -13825,7 +14867,7 @@
       </c>
       <c r="N174" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3e2683b8-ec61-9727-3b8b-f02554d1e4c3-20220423_172127.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=Bn8WslJlhWBb5rIn3RfDddbToOc</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F3e2683b8-ec61-9727-3b8b-f02554d1e4c3-20220423_172127.jpg?Expires=1652726495814&amp;KeyName=labelbox-assets-key-3&amp;Signature=Hxh7JUh9oDEGlD7yUNuVdZe2Acc</t>
         </is>
       </c>
       <c r="O174" t="inlineStr">
@@ -13840,9 +14882,15 @@
         <v>309</v>
       </c>
       <c r="R174" t="n">
+        <v>1310</v>
+      </c>
+      <c r="S174" t="n">
+        <v>1748</v>
+      </c>
+      <c r="T174" t="n">
         <v>0.9331210191082803</v>
       </c>
-      <c r="S174" t="n">
+      <c r="U174" t="n">
         <v>0.1120689655172413</v>
       </c>
     </row>
@@ -13902,7 +14950,7 @@
       </c>
       <c r="N175" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5198006-a46f-e29b-2fd5-5f4ee109599b-20220423_172131.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=xDw0YYlmetdXBAujSKVlXfFpvmk</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fd5198006-a46f-e29b-2fd5-5f4ee109599b-20220423_172131.jpg?Expires=1652726495814&amp;KeyName=labelbox-assets-key-3&amp;Signature=wLuhTnM-eZG8q15iJ1jjz1oLmWw</t>
         </is>
       </c>
       <c r="O175" t="inlineStr">
@@ -13917,9 +14965,15 @@
         <v>288</v>
       </c>
       <c r="R175" t="n">
+        <v>1315</v>
+      </c>
+      <c r="S175" t="n">
+        <v>1766</v>
+      </c>
+      <c r="T175" t="n">
         <v>0.9713375796178344</v>
       </c>
-      <c r="S175" t="n">
+      <c r="U175" t="n">
         <v>0.1724137931034483</v>
       </c>
     </row>
@@ -13979,7 +15033,7 @@
       </c>
       <c r="N176" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9283ccee-e4d7-a947-e445-b82b68fdcaae-20220423_172231.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=VME-oyLDR8q6VZvraI5Sn3t4Zm4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9283ccee-e4d7-a947-e445-b82b68fdcaae-20220423_172231.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=LfyoLPV-34kbBmbp1NrHcO1rnvo</t>
         </is>
       </c>
       <c r="O176" t="inlineStr">
@@ -13994,9 +15048,15 @@
         <v>386</v>
       </c>
       <c r="R176" t="n">
-        <v>0</v>
+        <v>1198</v>
       </c>
       <c r="S176" t="n">
+        <v>1633</v>
+      </c>
+      <c r="T176" t="n">
+        <v>0</v>
+      </c>
+      <c r="U176" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14056,7 +15116,7 @@
       </c>
       <c r="N177" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9283ccee-e4d7-a947-e445-b82b68fdcaae-20220423_172231.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=VME-oyLDR8q6VZvraI5Sn3t4Zm4</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9283ccee-e4d7-a947-e445-b82b68fdcaae-20220423_172231.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=LfyoLPV-34kbBmbp1NrHcO1rnvo</t>
         </is>
       </c>
       <c r="O177" t="inlineStr">
@@ -14071,9 +15131,15 @@
         <v>386</v>
       </c>
       <c r="R177" t="n">
-        <v>0</v>
+        <v>1198</v>
       </c>
       <c r="S177" t="n">
+        <v>1633</v>
+      </c>
+      <c r="T177" t="n">
+        <v>0</v>
+      </c>
+      <c r="U177" t="n">
         <v>0</v>
       </c>
     </row>
@@ -14133,7 +15199,7 @@
       </c>
       <c r="N178" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa022c2da-c3e7-3c7d-5906-1398d2bd22e3-20220423_172235.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=IUetnEoDaUUYaxCI5yQrdLc8R0g</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fa022c2da-c3e7-3c7d-5906-1398d2bd22e3-20220423_172235.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=QfsAIFlkdUtlHANwMr_53sMez6c</t>
         </is>
       </c>
       <c r="O178" t="inlineStr">
@@ -14148,9 +15214,15 @@
         <v>392</v>
       </c>
       <c r="R178" t="n">
+        <v>1274</v>
+      </c>
+      <c r="S178" t="n">
+        <v>1665</v>
+      </c>
+      <c r="T178" t="n">
         <v>0.6153846153846154</v>
       </c>
-      <c r="S178" t="n">
+      <c r="U178" t="n">
         <v>-0.01554404145077726</v>
       </c>
     </row>
@@ -14210,7 +15282,7 @@
       </c>
       <c r="N179" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9ef9d622-e54c-a384-29a5-4a30e48af4be-20220423_172239.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=267Ho_p_l67ALl1w8qz5NpfMw6o</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9ef9d622-e54c-a384-29a5-4a30e48af4be-20220423_172239.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=K2MhUiTrvHyS2EfqLBOdG4OvqbY</t>
         </is>
       </c>
       <c r="O179" t="inlineStr">
@@ -14225,9 +15297,15 @@
         <v>364</v>
       </c>
       <c r="R179" t="n">
+        <v>1296</v>
+      </c>
+      <c r="S179" t="n">
+        <v>1694</v>
+      </c>
+      <c r="T179" t="n">
         <v>0.7769230769230769</v>
       </c>
-      <c r="S179" t="n">
+      <c r="U179" t="n">
         <v>0.05699481865284972</v>
       </c>
     </row>
@@ -14287,7 +15365,7 @@
       </c>
       <c r="N180" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9a6ff8ee-19c8-833f-f1e2-0d4d5563652a-20220423_172242.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=fqDgODdRZh1Zu_Qyzbr-Ur7szbY</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F9a6ff8ee-19c8-833f-f1e2-0d4d5563652a-20220423_172242.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=-BPhPgw8xG1yzp7ysSHRbfz2nv0</t>
         </is>
       </c>
       <c r="O180" t="inlineStr">
@@ -14302,9 +15380,15 @@
         <v>335</v>
       </c>
       <c r="R180" t="n">
+        <v>1312</v>
+      </c>
+      <c r="S180" t="n">
+        <v>1724</v>
+      </c>
+      <c r="T180" t="n">
         <v>0.8846153846153846</v>
       </c>
-      <c r="S180" t="n">
+      <c r="U180" t="n">
         <v>0.1321243523316062</v>
       </c>
     </row>
@@ -14364,7 +15448,7 @@
       </c>
       <c r="N181" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F69d3267e-b6d9-31f9-5cf8-963ef4132e70-20220423_172246.jpg?Expires=1652401055970&amp;KeyName=labelbox-assets-key-3&amp;Signature=cWdbzJDVH9DZLiTyZyeqjlmAndQ</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2F69d3267e-b6d9-31f9-5cf8-963ef4132e70-20220423_172246.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=VDCaVv82YVlRhVMNlGOhgPGMj_c</t>
         </is>
       </c>
       <c r="O181" t="inlineStr">
@@ -14379,9 +15463,15 @@
         <v>307</v>
       </c>
       <c r="R181" t="n">
+        <v>1317</v>
+      </c>
+      <c r="S181" t="n">
+        <v>1747</v>
+      </c>
+      <c r="T181" t="n">
         <v>0.926923076923077</v>
       </c>
-      <c r="S181" t="n">
+      <c r="U181" t="n">
         <v>0.2046632124352331</v>
       </c>
     </row>
@@ -14441,7 +15531,7 @@
       </c>
       <c r="N182" t="inlineStr">
         <is>
-          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb95ae938-d4e8-0f5d-a2dd-d0d8d519db4d-20220423_172250.jpg?Expires=1652401055971&amp;KeyName=labelbox-assets-key-3&amp;Signature=AELfiVUHbxPK6e68yw3DfCrwey0</t>
+          <t>https://storage.labelbox.com/cl2ceiao35hbj0zahefxyfyll%2Fb95ae938-d4e8-0f5d-a2dd-d0d8d519db4d-20220423_172250.jpg?Expires=1652726495815&amp;KeyName=labelbox-assets-key-3&amp;Signature=BdIhja6m3VR4edZq4fjP95LuSMw</t>
         </is>
       </c>
       <c r="O182" t="inlineStr">
@@ -14456,9 +15546,15 @@
         <v>272</v>
       </c>
       <c r="R182" t="n">
+        <v>1323</v>
+      </c>
+      <c r="S182" t="n">
+        <v>1774</v>
+      </c>
+      <c r="T182" t="n">
         <v>0.9846153846153847</v>
       </c>
-      <c r="S182" t="n">
+      <c r="U182" t="n">
         <v>0.2953367875647669</v>
       </c>
     </row>

</xml_diff>